<commit_message>
RunType and Meshwidth added to Simparameters
</commit_message>
<xml_diff>
--- a/ParameterIndependent/InputSheet.xlsx
+++ b/ParameterIndependent/InputSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Code\Raytracer\ParameterIndependent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875F7623-DF0A-4251-98D4-57197672065E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DF6375-50B8-4C7C-9566-96F5A8810DD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AngleSpacing" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>Angles</t>
   </si>
@@ -115,9 +115,6 @@
     <t>z</t>
   </si>
   <si>
-    <t>Box Objects</t>
-  </si>
-  <si>
     <t>xmin</t>
   </si>
   <si>
@@ -149,6 +146,54 @@
   </si>
   <si>
     <t xml:space="preserve">Number of triangles on each surface of the box </t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>p0x</t>
+  </si>
+  <si>
+    <t>p0y</t>
+  </si>
+  <si>
+    <t>p0z</t>
+  </si>
+  <si>
+    <t>p1x</t>
+  </si>
+  <si>
+    <t>p1y</t>
+  </si>
+  <si>
+    <t>p1z</t>
+  </si>
+  <si>
+    <t>p2x</t>
+  </si>
+  <si>
+    <t>p2y</t>
+  </si>
+  <si>
+    <t>p2z</t>
+  </si>
+  <si>
+    <t>Meshwidth</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Runplottype</t>
+  </si>
+  <si>
+    <t>PerfectRefCentre</t>
+  </si>
+  <si>
+    <t>Change when LOS, PerfRef or Tx are changed</t>
   </si>
 </sst>
 </file>
@@ -265,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -279,10 +324,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -693,16 +734,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" style="7" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12" style="6" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="6" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -839,13 +881,32 @@
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -882,164 +943,212 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S1" sqref="K1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="2" max="4" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H1" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I1" t="s">
         <v>33</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3">
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>0.25</v>
       </c>
-      <c r="D3">
+      <c r="F2">
         <v>0.5</v>
       </c>
-      <c r="E3">
+      <c r="G2">
         <v>0.25</v>
       </c>
-      <c r="F3">
+      <c r="H2">
         <v>0.5</v>
       </c>
-      <c r="G3">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="J2">
         <v>0.25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BDEE68-C0E0-4A55-8CF0-A0DA678040E4}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="A1:H2"/>
+      <selection activeCell="K1" sqref="K1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="2" max="4" width="32.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:19" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H1" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I1" t="s">
         <v>33</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3">
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added check for whether the transmitter is inside an obstacle
</commit_message>
<xml_diff>
--- a/ParameterIndependent/InputSheet.xlsx
+++ b/ParameterIndependent/InputSheet.xlsx
@@ -29,6 +29,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Directions244" sheetId="20" state="visible" r:id="rId20"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Directions282" sheetId="21" state="visible" r:id="rId21"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Directions337" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Directions022" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -684,29 +685,29 @@
         <v>0</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="12">
       <c r="A3" s="11" t="n">
-        <v>0.3830222215594891</v>
+        <v>0.383022221559489</v>
       </c>
       <c r="B3" s="11" t="n">
-        <v>0.6634139481689384</v>
+        <v>0.663413948168938</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="12">
       <c r="A4" s="11" t="n">
-        <v>-0.3830222215594888</v>
+        <v>-0.383022221559489</v>
       </c>
       <c r="B4" s="11" t="n">
-        <v>0.6634139481689384</v>
+        <v>0.663413948168938</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="12">
@@ -714,32 +715,32 @@
         <v>-0.766044443118978</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>9.381338752702731e-17</v>
+        <v>9.38133875270273e-17</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="12">
       <c r="A6" s="11" t="n">
-        <v>-0.3830222215594893</v>
+        <v>-0.383022221559489</v>
       </c>
       <c r="B6" s="11" t="n">
-        <v>-0.6634139481689382</v>
+        <v>-0.663413948168938</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="12">
       <c r="A7" s="11" t="n">
-        <v>0.3830222215594885</v>
+        <v>0.383022221559489</v>
       </c>
       <c r="B7" s="11" t="n">
-        <v>-0.6634139481689387</v>
+        <v>-0.6634139481689389</v>
       </c>
       <c r="C7" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="12">
@@ -755,10 +756,10 @@
     </row>
     <row r="9" ht="15" customHeight="1" s="12">
       <c r="A9" s="11" t="n">
-        <v>0.7071067811865476</v>
+        <v>0.707106781186548</v>
       </c>
       <c r="B9" s="11" t="n">
-        <v>0.7071067811865475</v>
+        <v>0.707106781186547</v>
       </c>
       <c r="C9" s="11" t="n">
         <v>0</v>
@@ -766,7 +767,7 @@
     </row>
     <row r="10" ht="15" customHeight="1" s="12">
       <c r="A10" s="11" t="n">
-        <v>6.123233995736766e-17</v>
+        <v>6.12323399573677e-17</v>
       </c>
       <c r="B10" s="11" t="n">
         <v>1</v>
@@ -777,10 +778,10 @@
     </row>
     <row r="11" ht="15" customHeight="1" s="12">
       <c r="A11" s="11" t="n">
-        <v>-0.7071067811865475</v>
+        <v>-0.707106781186547</v>
       </c>
       <c r="B11" s="11" t="n">
-        <v>0.7071067811865476</v>
+        <v>0.707106781186548</v>
       </c>
       <c r="C11" s="11" t="n">
         <v>0</v>
@@ -791,7 +792,7 @@
         <v>-1</v>
       </c>
       <c r="B12" s="11" t="n">
-        <v>1.224646799147353e-16</v>
+        <v>1.22464679914735e-16</v>
       </c>
       <c r="C12" s="11" t="n">
         <v>0</v>
@@ -799,10 +800,10 @@
     </row>
     <row r="13" ht="15" customHeight="1" s="12">
       <c r="A13" s="11" t="n">
-        <v>-0.7071067811865477</v>
+        <v>-0.707106781186548</v>
       </c>
       <c r="B13" s="11" t="n">
-        <v>-0.7071067811865475</v>
+        <v>-0.707106781186547</v>
       </c>
       <c r="C13" s="11" t="n">
         <v>0</v>
@@ -821,10 +822,10 @@
     </row>
     <row r="15" ht="15" customHeight="1" s="12">
       <c r="A15" s="11" t="n">
-        <v>0.7071067811865474</v>
+        <v>0.707106781186547</v>
       </c>
       <c r="B15" s="11" t="n">
-        <v>-0.7071067811865477</v>
+        <v>-0.707106781186548</v>
       </c>
       <c r="C15" s="11" t="n">
         <v>0</v>
@@ -838,29 +839,29 @@
         <v>0</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="12">
       <c r="A17" s="11" t="n">
-        <v>0.3830222215594891</v>
+        <v>0.383022221559489</v>
       </c>
       <c r="B17" s="11" t="n">
-        <v>0.6634139481689384</v>
+        <v>0.663413948168938</v>
       </c>
       <c r="C17" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="12">
       <c r="A18" s="11" t="n">
-        <v>-0.3830222215594888</v>
+        <v>-0.383022221559489</v>
       </c>
       <c r="B18" s="11" t="n">
-        <v>0.6634139481689384</v>
+        <v>0.663413948168938</v>
       </c>
       <c r="C18" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="12">
@@ -868,32 +869,32 @@
         <v>-0.766044443118978</v>
       </c>
       <c r="B19" s="11" t="n">
-        <v>9.381338752702731e-17</v>
+        <v>9.38133875270273e-17</v>
       </c>
       <c r="C19" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="12">
       <c r="A20" s="11" t="n">
-        <v>-0.3830222215594893</v>
+        <v>-0.383022221559489</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>-0.6634139481689382</v>
+        <v>-0.663413948168938</v>
       </c>
       <c r="C20" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="12">
       <c r="A21" s="11" t="n">
-        <v>0.3830222215594885</v>
+        <v>0.383022221559489</v>
       </c>
       <c r="B21" s="11" t="n">
-        <v>-0.6634139481689387</v>
+        <v>-0.6634139481689389</v>
       </c>
       <c r="C21" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="12">
@@ -944,112 +945,112 @@
     </row>
     <row r="2" ht="15" customHeight="1" s="12">
       <c r="A2" s="11" t="n">
-        <v>0.3090169943749475</v>
+        <v>0.309016994374947</v>
       </c>
       <c r="B2" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>0.9510565162951535</v>
+        <v>0.951056516295153</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="12">
       <c r="A3" s="11" t="n">
-        <v>-0.3090169943749475</v>
+        <v>-0.309016994374947</v>
       </c>
       <c r="B3" s="11" t="n">
-        <v>3.784366730434151e-17</v>
+        <v>3.78436673043415e-17</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>0.9510565162951535</v>
+        <v>0.951056516295153</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="12">
       <c r="A4" s="11" t="n">
-        <v>0.8090169943749475</v>
+        <v>0.809016994374947</v>
       </c>
       <c r="B4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>0.5877852522924731</v>
+        <v>0.587785252292473</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="12">
       <c r="A5" s="11" t="n">
-        <v>0.5720614028176844</v>
+        <v>0.572061402817684</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>0.5720614028176843</v>
+        <v>0.572061402817684</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>0.5877852522924731</v>
+        <v>0.587785252292473</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="12">
       <c r="A6" s="11" t="n">
-        <v>4.953800363085458e-17</v>
+        <v>4.95380036308546e-17</v>
       </c>
       <c r="B6" s="11" t="n">
-        <v>0.8090169943749475</v>
+        <v>0.809016994374947</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>0.5877852522924731</v>
+        <v>0.587785252292473</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="12">
       <c r="A7" s="11" t="n">
-        <v>-0.5720614028176843</v>
+        <v>-0.572061402817684</v>
       </c>
       <c r="B7" s="11" t="n">
-        <v>0.5720614028176844</v>
+        <v>0.572061402817684</v>
       </c>
       <c r="C7" s="11" t="n">
-        <v>0.5877852522924731</v>
+        <v>0.587785252292473</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="12">
       <c r="A8" s="11" t="n">
-        <v>-0.8090169943749475</v>
+        <v>-0.809016994374947</v>
       </c>
       <c r="B8" s="11" t="n">
-        <v>9.907600726170916e-17</v>
+        <v>9.90760072617092e-17</v>
       </c>
       <c r="C8" s="11" t="n">
-        <v>0.5877852522924731</v>
+        <v>0.587785252292473</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="12">
       <c r="A9" s="11" t="n">
-        <v>-0.5720614028176845</v>
+        <v>-0.572061402817684</v>
       </c>
       <c r="B9" s="11" t="n">
-        <v>-0.5720614028176843</v>
+        <v>-0.572061402817684</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>0.5877852522924731</v>
+        <v>0.587785252292473</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="12">
       <c r="A10" s="11" t="n">
-        <v>-1.486140108925637e-16</v>
+        <v>-1.48614010892564e-16</v>
       </c>
       <c r="B10" s="11" t="n">
-        <v>-0.8090169943749475</v>
+        <v>-0.809016994374947</v>
       </c>
       <c r="C10" s="11" t="n">
-        <v>0.5877852522924731</v>
+        <v>0.587785252292473</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="12">
       <c r="A11" s="11" t="n">
-        <v>0.5720614028176841</v>
+        <v>0.572061402817684</v>
       </c>
       <c r="B11" s="11" t="n">
-        <v>-0.5720614028176845</v>
+        <v>-0.572061402817684</v>
       </c>
       <c r="C11" s="11" t="n">
-        <v>0.5877852522924731</v>
+        <v>0.587785252292473</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="12">
@@ -1065,10 +1066,10 @@
     </row>
     <row r="13" ht="15" customHeight="1" s="12">
       <c r="A13" s="11" t="n">
-        <v>0.8090169943749475</v>
+        <v>0.809016994374947</v>
       </c>
       <c r="B13" s="11" t="n">
-        <v>0.5877852522924731</v>
+        <v>0.587785252292473</v>
       </c>
       <c r="C13" s="11" t="n">
         <v>0</v>
@@ -1076,10 +1077,10 @@
     </row>
     <row r="14" ht="15" customHeight="1" s="12">
       <c r="A14" s="11" t="n">
-        <v>0.3090169943749475</v>
+        <v>0.309016994374947</v>
       </c>
       <c r="B14" s="11" t="n">
-        <v>0.9510565162951535</v>
+        <v>0.951056516295153</v>
       </c>
       <c r="C14" s="11" t="n">
         <v>0</v>
@@ -1087,10 +1088,10 @@
     </row>
     <row r="15" ht="15" customHeight="1" s="12">
       <c r="A15" s="11" t="n">
-        <v>-0.3090169943749473</v>
+        <v>-0.309016994374947</v>
       </c>
       <c r="B15" s="11" t="n">
-        <v>0.9510565162951536</v>
+        <v>0.951056516295153</v>
       </c>
       <c r="C15" s="11" t="n">
         <v>0</v>
@@ -1098,10 +1099,10 @@
     </row>
     <row r="16" ht="15" customHeight="1" s="12">
       <c r="A16" s="11" t="n">
-        <v>-0.8090169943749473</v>
+        <v>-0.809016994374947</v>
       </c>
       <c r="B16" s="11" t="n">
-        <v>0.5877852522924732</v>
+        <v>0.587785252292473</v>
       </c>
       <c r="C16" s="11" t="n">
         <v>0</v>
@@ -1112,7 +1113,7 @@
         <v>-1</v>
       </c>
       <c r="B17" s="11" t="n">
-        <v>1.224646799147353e-16</v>
+        <v>1.22464679914735e-16</v>
       </c>
       <c r="C17" s="11" t="n">
         <v>0</v>
@@ -1120,7 +1121,7 @@
     </row>
     <row r="18" ht="15" customHeight="1" s="12">
       <c r="A18" s="11" t="n">
-        <v>-0.8090169943749476</v>
+        <v>-0.809016994374947</v>
       </c>
       <c r="B18" s="11" t="n">
         <v>-0.587785252292473</v>
@@ -1131,10 +1132,10 @@
     </row>
     <row r="19" ht="15" customHeight="1" s="12">
       <c r="A19" s="11" t="n">
-        <v>-0.3090169943749476</v>
+        <v>-0.309016994374948</v>
       </c>
       <c r="B19" s="11" t="n">
-        <v>-0.9510565162951535</v>
+        <v>-0.951056516295153</v>
       </c>
       <c r="C19" s="11" t="n">
         <v>0</v>
@@ -1142,10 +1143,10 @@
     </row>
     <row r="20" ht="15" customHeight="1" s="12">
       <c r="A20" s="11" t="n">
-        <v>0.3090169943749472</v>
+        <v>0.309016994374947</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>-0.9510565162951536</v>
+        <v>-0.951056516295153</v>
       </c>
       <c r="C20" s="11" t="n">
         <v>0</v>
@@ -1153,10 +1154,10 @@
     </row>
     <row r="21" ht="15" customHeight="1" s="12">
       <c r="A21" s="11" t="n">
-        <v>0.8090169943749473</v>
+        <v>0.809016994374947</v>
       </c>
       <c r="B21" s="11" t="n">
-        <v>-0.5877852522924734</v>
+        <v>-0.587785252292473</v>
       </c>
       <c r="C21" s="11" t="n">
         <v>0</v>
@@ -1164,112 +1165,112 @@
     </row>
     <row r="22" ht="15" customHeight="1" s="12">
       <c r="A22" s="11" t="n">
-        <v>0.8090169943749475</v>
+        <v>0.809016994374947</v>
       </c>
       <c r="B22" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C22" s="11" t="n">
-        <v>-0.5877852522924731</v>
+        <v>-0.587785252292473</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="12">
       <c r="A23" s="11" t="n">
-        <v>0.5720614028176844</v>
+        <v>0.572061402817684</v>
       </c>
       <c r="B23" s="11" t="n">
-        <v>0.5720614028176843</v>
+        <v>0.572061402817684</v>
       </c>
       <c r="C23" s="11" t="n">
-        <v>-0.5877852522924731</v>
+        <v>-0.587785252292473</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="12">
       <c r="A24" s="11" t="n">
-        <v>4.953800363085458e-17</v>
+        <v>4.95380036308546e-17</v>
       </c>
       <c r="B24" s="11" t="n">
-        <v>0.8090169943749475</v>
+        <v>0.809016994374947</v>
       </c>
       <c r="C24" s="11" t="n">
-        <v>-0.5877852522924731</v>
+        <v>-0.587785252292473</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="12">
       <c r="A25" s="11" t="n">
-        <v>-0.5720614028176843</v>
+        <v>-0.572061402817684</v>
       </c>
       <c r="B25" s="11" t="n">
-        <v>0.5720614028176844</v>
+        <v>0.572061402817684</v>
       </c>
       <c r="C25" s="11" t="n">
-        <v>-0.5877852522924731</v>
+        <v>-0.587785252292473</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" s="12">
       <c r="A26" s="11" t="n">
-        <v>-0.8090169943749475</v>
+        <v>-0.809016994374947</v>
       </c>
       <c r="B26" s="11" t="n">
-        <v>9.907600726170916e-17</v>
+        <v>9.90760072617092e-17</v>
       </c>
       <c r="C26" s="11" t="n">
-        <v>-0.5877852522924731</v>
+        <v>-0.587785252292473</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="12">
       <c r="A27" s="11" t="n">
-        <v>-0.5720614028176845</v>
+        <v>-0.572061402817684</v>
       </c>
       <c r="B27" s="11" t="n">
-        <v>-0.5720614028176843</v>
+        <v>-0.572061402817684</v>
       </c>
       <c r="C27" s="11" t="n">
-        <v>-0.5877852522924731</v>
+        <v>-0.587785252292473</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" s="12">
       <c r="A28" s="11" t="n">
-        <v>-1.486140108925637e-16</v>
+        <v>-1.48614010892564e-16</v>
       </c>
       <c r="B28" s="11" t="n">
-        <v>-0.8090169943749475</v>
+        <v>-0.809016994374947</v>
       </c>
       <c r="C28" s="11" t="n">
-        <v>-0.5877852522924731</v>
+        <v>-0.587785252292473</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="12">
       <c r="A29" s="11" t="n">
-        <v>0.5720614028176841</v>
+        <v>0.572061402817684</v>
       </c>
       <c r="B29" s="11" t="n">
-        <v>-0.5720614028176845</v>
+        <v>-0.572061402817684</v>
       </c>
       <c r="C29" s="11" t="n">
-        <v>-0.5877852522924731</v>
+        <v>-0.587785252292473</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="12">
       <c r="A30" s="11" t="n">
-        <v>0.3090169943749475</v>
+        <v>0.309016994374947</v>
       </c>
       <c r="B30" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C30" s="11" t="n">
-        <v>-0.9510565162951535</v>
+        <v>-0.951056516295153</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" s="12">
       <c r="A31" s="11" t="n">
-        <v>-0.3090169943749475</v>
+        <v>-0.309016994374947</v>
       </c>
       <c r="B31" s="11" t="n">
-        <v>3.784366730434151e-17</v>
+        <v>3.78436673043415e-17</v>
       </c>
       <c r="C31" s="11" t="n">
-        <v>-0.9510565162951535</v>
+        <v>-0.951056516295153</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="12">
@@ -1320,167 +1321,167 @@
     </row>
     <row r="2" ht="15" customHeight="1" s="12">
       <c r="A2" s="11" t="n">
-        <v>0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="B2" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="12">
       <c r="A3" s="11" t="n">
-        <v>0.1545084971874738</v>
+        <v>0.154508497187474</v>
       </c>
       <c r="B3" s="11" t="n">
-        <v>0.4755282581475769</v>
+        <v>0.475528258147577</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="12">
       <c r="A4" s="11" t="n">
-        <v>-0.4045084971874738</v>
+        <v>-0.404508497187474</v>
       </c>
       <c r="B4" s="11" t="n">
-        <v>0.2938926261462367</v>
+        <v>0.293892626146237</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="12">
       <c r="A5" s="11" t="n">
-        <v>-0.4045084971874739</v>
+        <v>-0.404508497187474</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>-0.2938926261462366</v>
+        <v>-0.293892626146237</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="12">
       <c r="A6" s="11" t="n">
-        <v>0.1545084971874736</v>
+        <v>0.154508497187474</v>
       </c>
       <c r="B6" s="11" t="n">
-        <v>-0.4755282581475769</v>
+        <v>-0.475528258147577</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="12">
       <c r="A7" s="11" t="n">
-        <v>0.8660254037844387</v>
+        <v>0.866025403784439</v>
       </c>
       <c r="B7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="11" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="12">
       <c r="A8" s="11" t="n">
-        <v>0.7006292692220368</v>
+        <v>0.7006292692220371</v>
       </c>
       <c r="B8" s="11" t="n">
-        <v>0.5090369604551273</v>
+        <v>0.509036960455127</v>
       </c>
       <c r="C8" s="11" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="12">
       <c r="A9" s="11" t="n">
-        <v>0.2676165673298175</v>
+        <v>0.267616567329817</v>
       </c>
       <c r="B9" s="11" t="n">
         <v>0.823639103546332</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="12">
       <c r="A10" s="11" t="n">
-        <v>-0.2676165673298174</v>
+        <v>-0.267616567329817</v>
       </c>
       <c r="B10" s="11" t="n">
-        <v>0.8236391035463321</v>
+        <v>0.823639103546332</v>
       </c>
       <c r="C10" s="11" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="12">
       <c r="A11" s="11" t="n">
-        <v>-0.7006292692220367</v>
+        <v>-0.7006292692220371</v>
       </c>
       <c r="B11" s="11" t="n">
-        <v>0.5090369604551274</v>
+        <v>0.509036960455127</v>
       </c>
       <c r="C11" s="11" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="12">
       <c r="A12" s="11" t="n">
-        <v>-0.8660254037844387</v>
+        <v>-0.866025403784439</v>
       </c>
       <c r="B12" s="11" t="n">
-        <v>1.060575238724907e-16</v>
+        <v>1.06057523872491e-16</v>
       </c>
       <c r="C12" s="11" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="12">
       <c r="A13" s="11" t="n">
-        <v>-0.7006292692220369</v>
+        <v>-0.7006292692220371</v>
       </c>
       <c r="B13" s="11" t="n">
-        <v>-0.5090369604551271</v>
+        <v>-0.509036960455127</v>
       </c>
       <c r="C13" s="11" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="12">
       <c r="A14" s="11" t="n">
-        <v>-0.2676165673298176</v>
+        <v>-0.267616567329818</v>
       </c>
       <c r="B14" s="11" t="n">
         <v>-0.823639103546332</v>
       </c>
       <c r="C14" s="11" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="12">
       <c r="A15" s="11" t="n">
-        <v>0.2676165673298173</v>
+        <v>0.267616567329817</v>
       </c>
       <c r="B15" s="11" t="n">
-        <v>-0.8236391035463321</v>
+        <v>-0.823639103546332</v>
       </c>
       <c r="C15" s="11" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="12">
       <c r="A16" s="11" t="n">
-        <v>0.7006292692220367</v>
+        <v>0.7006292692220371</v>
       </c>
       <c r="B16" s="11" t="n">
-        <v>-0.5090369604551274</v>
+        <v>-0.509036960455127</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="12">
@@ -1496,10 +1497,10 @@
     </row>
     <row r="18" ht="15" customHeight="1" s="12">
       <c r="A18" s="11" t="n">
-        <v>0.8660254037844387</v>
+        <v>0.866025403784439</v>
       </c>
       <c r="B18" s="11" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="C18" s="11" t="n">
         <v>0</v>
@@ -1507,10 +1508,10 @@
     </row>
     <row r="19" ht="15" customHeight="1" s="12">
       <c r="A19" s="11" t="n">
-        <v>0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="B19" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
       <c r="C19" s="11" t="n">
         <v>0</v>
@@ -1518,7 +1519,7 @@
     </row>
     <row r="20" ht="15" customHeight="1" s="12">
       <c r="A20" s="11" t="n">
-        <v>6.123233995736766e-17</v>
+        <v>6.12323399573677e-17</v>
       </c>
       <c r="B20" s="11" t="n">
         <v>1</v>
@@ -1529,10 +1530,10 @@
     </row>
     <row r="21" ht="15" customHeight="1" s="12">
       <c r="A21" s="11" t="n">
-        <v>-0.4999999999999998</v>
+        <v>-0.5</v>
       </c>
       <c r="B21" s="11" t="n">
-        <v>0.8660254037844387</v>
+        <v>0.866025403784439</v>
       </c>
       <c r="C21" s="11" t="n">
         <v>0</v>
@@ -1540,10 +1541,10 @@
     </row>
     <row r="22" ht="15" customHeight="1" s="12">
       <c r="A22" s="11" t="n">
-        <v>-0.8660254037844385</v>
+        <v>-0.866025403784438</v>
       </c>
       <c r="B22" s="11" t="n">
-        <v>0.5000000000000003</v>
+        <v>0.5</v>
       </c>
       <c r="C22" s="11" t="n">
         <v>0</v>
@@ -1554,7 +1555,7 @@
         <v>-1</v>
       </c>
       <c r="B23" s="11" t="n">
-        <v>1.224646799147353e-16</v>
+        <v>1.22464679914735e-16</v>
       </c>
       <c r="C23" s="11" t="n">
         <v>0</v>
@@ -1562,10 +1563,10 @@
     </row>
     <row r="24" ht="15" customHeight="1" s="12">
       <c r="A24" s="11" t="n">
-        <v>-0.8660254037844388</v>
+        <v>-0.866025403784439</v>
       </c>
       <c r="B24" s="11" t="n">
-        <v>-0.4999999999999997</v>
+        <v>-0.5</v>
       </c>
       <c r="C24" s="11" t="n">
         <v>0</v>
@@ -1573,10 +1574,10 @@
     </row>
     <row r="25" ht="15" customHeight="1" s="12">
       <c r="A25" s="11" t="n">
-        <v>-0.5000000000000004</v>
+        <v>-0.5</v>
       </c>
       <c r="B25" s="11" t="n">
-        <v>-0.8660254037844384</v>
+        <v>-0.866025403784438</v>
       </c>
       <c r="C25" s="11" t="n">
         <v>0</v>
@@ -1595,7 +1596,7 @@
     </row>
     <row r="27" ht="15" customHeight="1" s="12">
       <c r="A27" s="11" t="n">
-        <v>0.4999999999999993</v>
+        <v>0.499999999999999</v>
       </c>
       <c r="B27" s="11" t="n">
         <v>-0.866025403784439</v>
@@ -1606,10 +1607,10 @@
     </row>
     <row r="28" ht="15" customHeight="1" s="12">
       <c r="A28" s="11" t="n">
-        <v>0.8660254037844384</v>
+        <v>0.866025403784438</v>
       </c>
       <c r="B28" s="11" t="n">
-        <v>-0.5000000000000004</v>
+        <v>-0.5</v>
       </c>
       <c r="C28" s="11" t="n">
         <v>0</v>
@@ -1617,167 +1618,167 @@
     </row>
     <row r="29" ht="15" customHeight="1" s="12">
       <c r="A29" s="11" t="n">
-        <v>0.8660254037844387</v>
+        <v>0.866025403784439</v>
       </c>
       <c r="B29" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C29" s="11" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="12">
       <c r="A30" s="11" t="n">
-        <v>0.7006292692220368</v>
+        <v>0.7006292692220371</v>
       </c>
       <c r="B30" s="11" t="n">
-        <v>0.5090369604551273</v>
+        <v>0.509036960455127</v>
       </c>
       <c r="C30" s="11" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" s="12">
       <c r="A31" s="11" t="n">
-        <v>0.2676165673298175</v>
+        <v>0.267616567329817</v>
       </c>
       <c r="B31" s="11" t="n">
         <v>0.823639103546332</v>
       </c>
       <c r="C31" s="11" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="12">
       <c r="A32" s="11" t="n">
-        <v>-0.2676165673298174</v>
+        <v>-0.267616567329817</v>
       </c>
       <c r="B32" s="11" t="n">
-        <v>0.8236391035463321</v>
+        <v>0.823639103546332</v>
       </c>
       <c r="C32" s="11" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="12">
       <c r="A33" s="11" t="n">
-        <v>-0.7006292692220367</v>
+        <v>-0.7006292692220371</v>
       </c>
       <c r="B33" s="11" t="n">
-        <v>0.5090369604551274</v>
+        <v>0.509036960455127</v>
       </c>
       <c r="C33" s="11" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="12">
       <c r="A34" s="11" t="n">
-        <v>-0.8660254037844387</v>
+        <v>-0.866025403784439</v>
       </c>
       <c r="B34" s="11" t="n">
-        <v>1.060575238724907e-16</v>
+        <v>1.06057523872491e-16</v>
       </c>
       <c r="C34" s="11" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="12">
       <c r="A35" s="11" t="n">
-        <v>-0.7006292692220369</v>
+        <v>-0.7006292692220371</v>
       </c>
       <c r="B35" s="11" t="n">
-        <v>-0.5090369604551271</v>
+        <v>-0.509036960455127</v>
       </c>
       <c r="C35" s="11" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" s="12">
       <c r="A36" s="11" t="n">
-        <v>-0.2676165673298176</v>
+        <v>-0.267616567329818</v>
       </c>
       <c r="B36" s="11" t="n">
         <v>-0.823639103546332</v>
       </c>
       <c r="C36" s="11" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="12">
       <c r="A37" s="11" t="n">
-        <v>0.2676165673298173</v>
+        <v>0.267616567329817</v>
       </c>
       <c r="B37" s="11" t="n">
-        <v>-0.8236391035463321</v>
+        <v>-0.823639103546332</v>
       </c>
       <c r="C37" s="11" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="12">
       <c r="A38" s="11" t="n">
-        <v>0.7006292692220367</v>
+        <v>0.7006292692220371</v>
       </c>
       <c r="B38" s="11" t="n">
-        <v>-0.5090369604551274</v>
+        <v>-0.509036960455127</v>
       </c>
       <c r="C38" s="11" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="12">
       <c r="A39" s="11" t="n">
-        <v>0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="B39" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C39" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="12">
       <c r="A40" s="11" t="n">
-        <v>0.1545084971874738</v>
+        <v>0.154508497187474</v>
       </c>
       <c r="B40" s="11" t="n">
-        <v>0.4755282581475769</v>
+        <v>0.475528258147577</v>
       </c>
       <c r="C40" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="12">
       <c r="A41" s="11" t="n">
-        <v>-0.4045084971874738</v>
+        <v>-0.404508497187474</v>
       </c>
       <c r="B41" s="11" t="n">
-        <v>0.2938926261462367</v>
+        <v>0.293892626146237</v>
       </c>
       <c r="C41" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="12">
       <c r="A42" s="11" t="n">
-        <v>-0.4045084971874739</v>
+        <v>-0.404508497187474</v>
       </c>
       <c r="B42" s="11" t="n">
-        <v>-0.2938926261462366</v>
+        <v>-0.293892626146237</v>
       </c>
       <c r="C42" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="12">
       <c r="A43" s="11" t="n">
-        <v>0.1545084971874736</v>
+        <v>0.154508497187474</v>
       </c>
       <c r="B43" s="11" t="n">
-        <v>-0.4755282581475769</v>
+        <v>-0.475528258147577</v>
       </c>
       <c r="C43" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="12">
@@ -1828,145 +1829,145 @@
     </row>
     <row r="2" ht="15" customHeight="1" s="12">
       <c r="A2" s="11" t="n">
-        <v>0.6234898018587336</v>
+        <v>0.623489801858734</v>
       </c>
       <c r="B2" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>0.7818314824680298</v>
+        <v>0.78183148246803</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="12">
       <c r="A3" s="11" t="n">
-        <v>0.4408738668949674</v>
+        <v>0.440873866894967</v>
       </c>
       <c r="B3" s="11" t="n">
-        <v>0.4408738668949674</v>
+        <v>0.440873866894967</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>0.7818314824680298</v>
+        <v>0.78183148246803</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="12">
       <c r="A4" s="11" t="n">
-        <v>3.817773950736578e-17</v>
+        <v>3.81777395073658e-17</v>
       </c>
       <c r="B4" s="11" t="n">
-        <v>0.6234898018587336</v>
+        <v>0.623489801858734</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>0.7818314824680298</v>
+        <v>0.78183148246803</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="12">
       <c r="A5" s="11" t="n">
-        <v>-0.4408738668949674</v>
+        <v>-0.440873866894967</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>0.4408738668949674</v>
+        <v>0.440873866894967</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>0.7818314824680298</v>
+        <v>0.78183148246803</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="12">
       <c r="A6" s="11" t="n">
-        <v>-0.6234898018587336</v>
+        <v>-0.623489801858734</v>
       </c>
       <c r="B6" s="11" t="n">
-        <v>7.635547901473156e-17</v>
+        <v>7.63554790147316e-17</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>0.7818314824680298</v>
+        <v>0.78183148246803</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="12">
       <c r="A7" s="11" t="n">
-        <v>-0.4408738668949675</v>
+        <v>-0.440873866894968</v>
       </c>
       <c r="B7" s="11" t="n">
-        <v>-0.4408738668949674</v>
+        <v>-0.440873866894967</v>
       </c>
       <c r="C7" s="11" t="n">
-        <v>0.7818314824680298</v>
+        <v>0.78183148246803</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="12">
       <c r="A8" s="11" t="n">
-        <v>-1.145332185220973e-16</v>
+        <v>-1.14533218522097e-16</v>
       </c>
       <c r="B8" s="11" t="n">
-        <v>-0.6234898018587336</v>
+        <v>-0.623489801858734</v>
       </c>
       <c r="C8" s="11" t="n">
-        <v>0.7818314824680298</v>
+        <v>0.78183148246803</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="12">
       <c r="A9" s="11" t="n">
-        <v>0.4408738668949673</v>
+        <v>0.440873866894967</v>
       </c>
       <c r="B9" s="11" t="n">
-        <v>-0.4408738668949675</v>
+        <v>-0.440873866894968</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>0.7818314824680298</v>
+        <v>0.78183148246803</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="12">
       <c r="A10" s="11" t="n">
-        <v>0.9009688679024191</v>
+        <v>0.900968867902419</v>
       </c>
       <c r="B10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C10" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="12">
       <c r="A11" s="11" t="n">
-        <v>0.7802619276224012</v>
+        <v>0.780261927622401</v>
       </c>
       <c r="B11" s="11" t="n">
-        <v>0.4504844339512095</v>
+        <v>0.45048443395121</v>
       </c>
       <c r="C11" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="12">
       <c r="A12" s="11" t="n">
-        <v>0.4504844339512097</v>
+        <v>0.45048443395121</v>
       </c>
       <c r="B12" s="11" t="n">
-        <v>0.7802619276224011</v>
+        <v>0.780261927622401</v>
       </c>
       <c r="C12" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="12">
       <c r="A13" s="11" t="n">
-        <v>5.516843201040561e-17</v>
+        <v>5.51684320104056e-17</v>
       </c>
       <c r="B13" s="11" t="n">
-        <v>0.9009688679024191</v>
+        <v>0.900968867902419</v>
       </c>
       <c r="C13" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="12">
       <c r="A14" s="11" t="n">
-        <v>-0.4504844339512094</v>
+        <v>-0.450484433951209</v>
       </c>
       <c r="B14" s="11" t="n">
-        <v>0.7802619276224012</v>
+        <v>0.780261927622401</v>
       </c>
       <c r="C14" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="12">
@@ -1974,32 +1975,32 @@
         <v>-0.780261927622401</v>
       </c>
       <c r="B15" s="11" t="n">
-        <v>0.4504844339512099</v>
+        <v>0.45048443395121</v>
       </c>
       <c r="C15" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="12">
       <c r="A16" s="11" t="n">
-        <v>-0.9009688679024191</v>
+        <v>-0.900968867902419</v>
       </c>
       <c r="B16" s="11" t="n">
-        <v>1.103368640208112e-16</v>
+        <v>1.10336864020811e-16</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="12">
       <c r="A17" s="11" t="n">
-        <v>-0.7802619276224012</v>
+        <v>-0.780261927622401</v>
       </c>
       <c r="B17" s="11" t="n">
-        <v>-0.4504844339512093</v>
+        <v>-0.450484433951209</v>
       </c>
       <c r="C17" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="12">
@@ -2007,21 +2008,21 @@
         <v>-0.45048443395121</v>
       </c>
       <c r="B18" s="11" t="n">
-        <v>-0.7802619276224009</v>
+        <v>-0.780261927622401</v>
       </c>
       <c r="C18" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="12">
       <c r="A19" s="11" t="n">
-        <v>-1.655052960312168e-16</v>
+        <v>-1.65505296031217e-16</v>
       </c>
       <c r="B19" s="11" t="n">
-        <v>-0.9009688679024191</v>
+        <v>-0.900968867902419</v>
       </c>
       <c r="C19" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="12">
@@ -2029,21 +2030,21 @@
         <v>0.450484433951209</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>-0.7802619276224014</v>
+        <v>-0.780261927622401</v>
       </c>
       <c r="C20" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="12">
       <c r="A21" s="11" t="n">
-        <v>0.7802619276224009</v>
+        <v>0.780261927622401</v>
       </c>
       <c r="B21" s="11" t="n">
         <v>-0.45048443395121</v>
       </c>
       <c r="C21" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="12">
@@ -2059,10 +2060,10 @@
     </row>
     <row r="23" ht="15" customHeight="1" s="12">
       <c r="A23" s="11" t="n">
-        <v>0.9009688679024191</v>
+        <v>0.900968867902419</v>
       </c>
       <c r="B23" s="11" t="n">
-        <v>0.4338837391175581</v>
+        <v>0.433883739117558</v>
       </c>
       <c r="C23" s="11" t="n">
         <v>0</v>
@@ -2070,10 +2071,10 @@
     </row>
     <row r="24" ht="15" customHeight="1" s="12">
       <c r="A24" s="11" t="n">
-        <v>0.6234898018587336</v>
+        <v>0.623489801858734</v>
       </c>
       <c r="B24" s="11" t="n">
-        <v>0.7818314824680298</v>
+        <v>0.78183148246803</v>
       </c>
       <c r="C24" s="11" t="n">
         <v>0</v>
@@ -2081,10 +2082,10 @@
     </row>
     <row r="25" ht="15" customHeight="1" s="12">
       <c r="A25" s="11" t="n">
-        <v>0.2225209339563144</v>
+        <v>0.222520933956314</v>
       </c>
       <c r="B25" s="11" t="n">
-        <v>0.9749279121818236</v>
+        <v>0.974927912181824</v>
       </c>
       <c r="C25" s="11" t="n">
         <v>0</v>
@@ -2092,10 +2093,10 @@
     </row>
     <row r="26" ht="15" customHeight="1" s="12">
       <c r="A26" s="11" t="n">
-        <v>-0.2225209339563143</v>
+        <v>-0.222520933956314</v>
       </c>
       <c r="B26" s="11" t="n">
-        <v>0.9749279121818236</v>
+        <v>0.974927912181824</v>
       </c>
       <c r="C26" s="11" t="n">
         <v>0</v>
@@ -2103,10 +2104,10 @@
     </row>
     <row r="27" ht="15" customHeight="1" s="12">
       <c r="A27" s="11" t="n">
-        <v>-0.6234898018587335</v>
+        <v>-0.623489801858733</v>
       </c>
       <c r="B27" s="11" t="n">
-        <v>0.7818314824680299</v>
+        <v>0.78183148246803</v>
       </c>
       <c r="C27" s="11" t="n">
         <v>0</v>
@@ -2117,7 +2118,7 @@
         <v>-0.900968867902419</v>
       </c>
       <c r="B28" s="11" t="n">
-        <v>0.4338837391175582</v>
+        <v>0.433883739117558</v>
       </c>
       <c r="C28" s="11" t="n">
         <v>0</v>
@@ -2128,7 +2129,7 @@
         <v>-1</v>
       </c>
       <c r="B29" s="11" t="n">
-        <v>1.224646799147353e-16</v>
+        <v>1.22464679914735e-16</v>
       </c>
       <c r="C29" s="11" t="n">
         <v>0</v>
@@ -2136,7 +2137,7 @@
     </row>
     <row r="30" ht="15" customHeight="1" s="12">
       <c r="A30" s="11" t="n">
-        <v>-0.9009688679024191</v>
+        <v>-0.900968867902419</v>
       </c>
       <c r="B30" s="11" t="n">
         <v>-0.433883739117558</v>
@@ -2147,10 +2148,10 @@
     </row>
     <row r="31" ht="15" customHeight="1" s="12">
       <c r="A31" s="11" t="n">
-        <v>-0.6234898018587337</v>
+        <v>-0.623489801858734</v>
       </c>
       <c r="B31" s="11" t="n">
-        <v>-0.7818314824680297</v>
+        <v>-0.78183148246803</v>
       </c>
       <c r="C31" s="11" t="n">
         <v>0</v>
@@ -2158,10 +2159,10 @@
     </row>
     <row r="32" ht="15" customHeight="1" s="12">
       <c r="A32" s="11" t="n">
-        <v>-0.2225209339563146</v>
+        <v>-0.222520933956315</v>
       </c>
       <c r="B32" s="11" t="n">
-        <v>-0.9749279121818236</v>
+        <v>-0.974927912181824</v>
       </c>
       <c r="C32" s="11" t="n">
         <v>0</v>
@@ -2169,10 +2170,10 @@
     </row>
     <row r="33" ht="15" customHeight="1" s="12">
       <c r="A33" s="11" t="n">
-        <v>0.2225209339563142</v>
+        <v>0.222520933956314</v>
       </c>
       <c r="B33" s="11" t="n">
-        <v>-0.9749279121818236</v>
+        <v>-0.974927912181824</v>
       </c>
       <c r="C33" s="11" t="n">
         <v>0</v>
@@ -2180,10 +2181,10 @@
     </row>
     <row r="34" ht="15" customHeight="1" s="12">
       <c r="A34" s="11" t="n">
-        <v>0.6234898018587334</v>
+        <v>0.623489801858733</v>
       </c>
       <c r="B34" s="11" t="n">
-        <v>-0.7818314824680299</v>
+        <v>-0.78183148246803</v>
       </c>
       <c r="C34" s="11" t="n">
         <v>0</v>
@@ -2194,7 +2195,7 @@
         <v>0.900968867902419</v>
       </c>
       <c r="B35" s="11" t="n">
-        <v>-0.4338837391175583</v>
+        <v>-0.433883739117558</v>
       </c>
       <c r="C35" s="11" t="n">
         <v>0</v>
@@ -2202,57 +2203,57 @@
     </row>
     <row r="36" ht="15" customHeight="1" s="12">
       <c r="A36" s="11" t="n">
-        <v>0.9009688679024191</v>
+        <v>0.900968867902419</v>
       </c>
       <c r="B36" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C36" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="12">
       <c r="A37" s="11" t="n">
-        <v>0.7802619276224012</v>
+        <v>0.780261927622401</v>
       </c>
       <c r="B37" s="11" t="n">
-        <v>0.4504844339512095</v>
+        <v>0.45048443395121</v>
       </c>
       <c r="C37" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="12">
       <c r="A38" s="11" t="n">
-        <v>0.4504844339512097</v>
+        <v>0.45048443395121</v>
       </c>
       <c r="B38" s="11" t="n">
-        <v>0.7802619276224011</v>
+        <v>0.780261927622401</v>
       </c>
       <c r="C38" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="12">
       <c r="A39" s="11" t="n">
-        <v>5.516843201040561e-17</v>
+        <v>5.51684320104056e-17</v>
       </c>
       <c r="B39" s="11" t="n">
-        <v>0.9009688679024191</v>
+        <v>0.900968867902419</v>
       </c>
       <c r="C39" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="12">
       <c r="A40" s="11" t="n">
-        <v>-0.4504844339512094</v>
+        <v>-0.450484433951209</v>
       </c>
       <c r="B40" s="11" t="n">
-        <v>0.7802619276224012</v>
+        <v>0.780261927622401</v>
       </c>
       <c r="C40" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="12">
@@ -2260,32 +2261,32 @@
         <v>-0.780261927622401</v>
       </c>
       <c r="B41" s="11" t="n">
-        <v>0.4504844339512099</v>
+        <v>0.45048443395121</v>
       </c>
       <c r="C41" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="12">
       <c r="A42" s="11" t="n">
-        <v>-0.9009688679024191</v>
+        <v>-0.900968867902419</v>
       </c>
       <c r="B42" s="11" t="n">
-        <v>1.103368640208112e-16</v>
+        <v>1.10336864020811e-16</v>
       </c>
       <c r="C42" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="12">
       <c r="A43" s="11" t="n">
-        <v>-0.7802619276224012</v>
+        <v>-0.780261927622401</v>
       </c>
       <c r="B43" s="11" t="n">
-        <v>-0.4504844339512093</v>
+        <v>-0.450484433951209</v>
       </c>
       <c r="C43" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="12">
@@ -2293,21 +2294,21 @@
         <v>-0.45048443395121</v>
       </c>
       <c r="B44" s="11" t="n">
-        <v>-0.7802619276224009</v>
+        <v>-0.780261927622401</v>
       </c>
       <c r="C44" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="12">
       <c r="A45" s="11" t="n">
-        <v>-1.655052960312168e-16</v>
+        <v>-1.65505296031217e-16</v>
       </c>
       <c r="B45" s="11" t="n">
-        <v>-0.9009688679024191</v>
+        <v>-0.900968867902419</v>
       </c>
       <c r="C45" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" s="12">
@@ -2315,109 +2316,109 @@
         <v>0.450484433951209</v>
       </c>
       <c r="B46" s="11" t="n">
-        <v>-0.7802619276224014</v>
+        <v>-0.780261927622401</v>
       </c>
       <c r="C46" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="12">
       <c r="A47" s="11" t="n">
-        <v>0.7802619276224009</v>
+        <v>0.780261927622401</v>
       </c>
       <c r="B47" s="11" t="n">
         <v>-0.45048443395121</v>
       </c>
       <c r="C47" s="11" t="n">
-        <v>-0.4338837391175581</v>
+        <v>-0.433883739117558</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="12">
       <c r="A48" s="11" t="n">
-        <v>0.6234898018587336</v>
+        <v>0.623489801858734</v>
       </c>
       <c r="B48" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C48" s="11" t="n">
-        <v>-0.7818314824680298</v>
+        <v>-0.78183148246803</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="12">
       <c r="A49" s="11" t="n">
-        <v>0.4408738668949674</v>
+        <v>0.440873866894967</v>
       </c>
       <c r="B49" s="11" t="n">
-        <v>0.4408738668949674</v>
+        <v>0.440873866894967</v>
       </c>
       <c r="C49" s="11" t="n">
-        <v>-0.7818314824680298</v>
+        <v>-0.78183148246803</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" s="12">
       <c r="A50" s="11" t="n">
-        <v>3.817773950736578e-17</v>
+        <v>3.81777395073658e-17</v>
       </c>
       <c r="B50" s="11" t="n">
-        <v>0.6234898018587336</v>
+        <v>0.623489801858734</v>
       </c>
       <c r="C50" s="11" t="n">
-        <v>-0.7818314824680298</v>
+        <v>-0.78183148246803</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" s="12">
       <c r="A51" s="11" t="n">
-        <v>-0.4408738668949674</v>
+        <v>-0.440873866894967</v>
       </c>
       <c r="B51" s="11" t="n">
-        <v>0.4408738668949674</v>
+        <v>0.440873866894967</v>
       </c>
       <c r="C51" s="11" t="n">
-        <v>-0.7818314824680298</v>
+        <v>-0.78183148246803</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="12">
       <c r="A52" s="11" t="n">
-        <v>-0.6234898018587336</v>
+        <v>-0.623489801858734</v>
       </c>
       <c r="B52" s="11" t="n">
-        <v>7.635547901473156e-17</v>
+        <v>7.63554790147316e-17</v>
       </c>
       <c r="C52" s="11" t="n">
-        <v>-0.7818314824680298</v>
+        <v>-0.78183148246803</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" s="12">
       <c r="A53" s="11" t="n">
-        <v>-0.4408738668949675</v>
+        <v>-0.440873866894968</v>
       </c>
       <c r="B53" s="11" t="n">
-        <v>-0.4408738668949674</v>
+        <v>-0.440873866894967</v>
       </c>
       <c r="C53" s="11" t="n">
-        <v>-0.7818314824680298</v>
+        <v>-0.78183148246803</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="12">
       <c r="A54" s="11" t="n">
-        <v>-1.145332185220973e-16</v>
+        <v>-1.14533218522097e-16</v>
       </c>
       <c r="B54" s="11" t="n">
-        <v>-0.6234898018587336</v>
+        <v>-0.623489801858734</v>
       </c>
       <c r="C54" s="11" t="n">
-        <v>-0.7818314824680298</v>
+        <v>-0.78183148246803</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="12">
       <c r="A55" s="11" t="n">
-        <v>0.4408738668949673</v>
+        <v>0.440873866894967</v>
       </c>
       <c r="B55" s="11" t="n">
-        <v>-0.4408738668949675</v>
+        <v>-0.440873866894968</v>
       </c>
       <c r="C55" s="11" t="n">
-        <v>-0.7818314824680298</v>
+        <v>-0.78183148246803</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="12">
@@ -2468,189 +2469,189 @@
     </row>
     <row r="2" ht="15" customHeight="1" s="12">
       <c r="A2" s="11" t="n">
-        <v>0.4457383557765383</v>
+        <v>0.445738355776538</v>
       </c>
       <c r="B2" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>0.8951632913550623</v>
+        <v>0.895163291355062</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="12">
       <c r="A3" s="11" t="n">
-        <v>0.2779133191239516</v>
+        <v>0.277913319123952</v>
       </c>
       <c r="B3" s="11" t="n">
         <v>0.348492279489633</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>0.8951632913550623</v>
+        <v>0.895163291355062</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="12">
       <c r="A4" s="11" t="n">
-        <v>-0.09918611522754722</v>
+        <v>-0.09918611522754719</v>
       </c>
       <c r="B4" s="11" t="n">
-        <v>0.4345627645765794</v>
+        <v>0.434562764576579</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>0.8951632913550623</v>
+        <v>0.895163291355062</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="12">
       <c r="A5" s="11" t="n">
-        <v>-0.4015963817846734</v>
+        <v>-0.401596381784673</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>0.1933986244724369</v>
+        <v>0.193398624472437</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>0.8951632913550623</v>
+        <v>0.895163291355062</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="12">
       <c r="A6" s="11" t="n">
-        <v>-0.4015963817846734</v>
+        <v>-0.401596381784673</v>
       </c>
       <c r="B6" s="11" t="n">
-        <v>-0.1933986244724368</v>
+        <v>-0.193398624472437</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>0.8951632913550623</v>
+        <v>0.895163291355062</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="12">
       <c r="A7" s="11" t="n">
-        <v>-0.09918611522754733</v>
+        <v>-0.09918611522754731</v>
       </c>
       <c r="B7" s="11" t="n">
-        <v>-0.4345627645765794</v>
+        <v>-0.434562764576579</v>
       </c>
       <c r="C7" s="11" t="n">
-        <v>0.8951632913550623</v>
+        <v>0.895163291355062</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="12">
       <c r="A8" s="11" t="n">
-        <v>0.2779133191239515</v>
+        <v>0.277913319123951</v>
       </c>
       <c r="B8" s="11" t="n">
-        <v>-0.3484922794896331</v>
+        <v>-0.348492279489633</v>
       </c>
       <c r="C8" s="11" t="n">
-        <v>0.8951632913550623</v>
+        <v>0.895163291355062</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="12">
       <c r="A9" s="11" t="n">
-        <v>0.7390089172206591</v>
+        <v>0.739008917220659</v>
       </c>
       <c r="B9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="12">
       <c r="A10" s="11" t="n">
-        <v>0.6400004959363221</v>
+        <v>0.640000495936322</v>
       </c>
       <c r="B10" s="11" t="n">
-        <v>0.3695044586103295</v>
+        <v>0.369504458610329</v>
       </c>
       <c r="C10" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="12">
       <c r="A11" s="11" t="n">
-        <v>0.3695044586103296</v>
+        <v>0.36950445861033</v>
       </c>
       <c r="B11" s="11" t="n">
         <v>0.640000495936322</v>
       </c>
       <c r="C11" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="12">
       <c r="A12" s="11" t="n">
-        <v>4.525124525078157e-17</v>
+        <v>4.52512452507816e-17</v>
       </c>
       <c r="B12" s="11" t="n">
-        <v>0.7390089172206591</v>
+        <v>0.739008917220659</v>
       </c>
       <c r="C12" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="12">
       <c r="A13" s="11" t="n">
-        <v>-0.3695044586103294</v>
+        <v>-0.369504458610329</v>
       </c>
       <c r="B13" s="11" t="n">
-        <v>0.6400004959363221</v>
+        <v>0.640000495936322</v>
       </c>
       <c r="C13" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="12">
       <c r="A14" s="11" t="n">
-        <v>-0.6400004959363219</v>
+        <v>-0.640000495936322</v>
       </c>
       <c r="B14" s="11" t="n">
-        <v>0.3695044586103298</v>
+        <v>0.36950445861033</v>
       </c>
       <c r="C14" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="12">
       <c r="A15" s="11" t="n">
-        <v>-0.7390089172206591</v>
+        <v>-0.739008917220659</v>
       </c>
       <c r="B15" s="11" t="n">
-        <v>9.050249050156315e-17</v>
+        <v>9.05024905015632e-17</v>
       </c>
       <c r="C15" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="12">
       <c r="A16" s="11" t="n">
-        <v>-0.6400004959363222</v>
+        <v>-0.640000495936322</v>
       </c>
       <c r="B16" s="11" t="n">
-        <v>-0.3695044586103293</v>
+        <v>-0.369504458610329</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="12">
       <c r="A17" s="11" t="n">
-        <v>-0.3695044586103299</v>
+        <v>-0.36950445861033</v>
       </c>
       <c r="B17" s="11" t="n">
-        <v>-0.6400004959363219</v>
+        <v>-0.640000495936322</v>
       </c>
       <c r="C17" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="12">
       <c r="A18" s="11" t="n">
-        <v>-1.357537357523447e-16</v>
+        <v>-1.35753735752345e-16</v>
       </c>
       <c r="B18" s="11" t="n">
-        <v>-0.7390089172206591</v>
+        <v>-0.739008917220659</v>
       </c>
       <c r="C18" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="12">
@@ -2658,43 +2659,43 @@
         <v>0.369504458610329</v>
       </c>
       <c r="B19" s="11" t="n">
-        <v>-0.6400004959363224</v>
+        <v>-0.640000495936322</v>
       </c>
       <c r="C19" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="12">
       <c r="A20" s="11" t="n">
-        <v>0.6400004959363219</v>
+        <v>0.640000495936322</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>-0.3695044586103299</v>
+        <v>-0.36950445861033</v>
       </c>
       <c r="C20" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="12">
       <c r="A21" s="11" t="n">
-        <v>0.9324722294043558</v>
+        <v>0.932472229404356</v>
       </c>
       <c r="B21" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C21" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="12">
       <c r="A22" s="11" t="n">
-        <v>0.8518557695502186</v>
+        <v>0.851855769550219</v>
       </c>
       <c r="B22" s="11" t="n">
-        <v>0.3792706243493351</v>
+        <v>0.379270624349335</v>
       </c>
       <c r="C22" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="12">
@@ -2702,142 +2703,142 @@
         <v>0.623945708274133</v>
       </c>
       <c r="B23" s="11" t="n">
-        <v>0.6929619121832167</v>
+        <v>0.692961912183217</v>
       </c>
       <c r="C23" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="12">
       <c r="A24" s="11" t="n">
-        <v>0.2881497656686405</v>
+        <v>0.28814976566864</v>
       </c>
       <c r="B24" s="11" t="n">
-        <v>0.8868337900392819</v>
+        <v>0.886833790039282</v>
       </c>
       <c r="C24" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="12">
       <c r="A25" s="11" t="n">
-        <v>-0.09746988917940001</v>
+        <v>-0.0974698891794</v>
       </c>
       <c r="B25" s="11" t="n">
-        <v>0.9273640489654994</v>
+        <v>0.927364048965499</v>
       </c>
       <c r="C25" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" s="12">
       <c r="A26" s="11" t="n">
-        <v>-0.4662361147021777</v>
+        <v>-0.466236114702178</v>
       </c>
       <c r="B26" s="11" t="n">
         <v>0.807544638987683</v>
       </c>
       <c r="C26" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="12">
       <c r="A27" s="11" t="n">
-        <v>-0.7543858803708183</v>
+        <v>-0.754385880370818</v>
       </c>
       <c r="B27" s="11" t="n">
-        <v>0.5480934246161643</v>
+        <v>0.5480934246161639</v>
       </c>
       <c r="C27" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" s="12">
       <c r="A28" s="11" t="n">
-        <v>-0.9120954739427733</v>
+        <v>-0.912095473942773</v>
       </c>
       <c r="B28" s="11" t="n">
-        <v>0.1938718778560655</v>
+        <v>0.193871877856065</v>
       </c>
       <c r="C28" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="12">
       <c r="A29" s="11" t="n">
-        <v>-0.9120954739427735</v>
+        <v>-0.912095473942773</v>
       </c>
       <c r="B29" s="11" t="n">
-        <v>-0.1938718778560649</v>
+        <v>-0.193871877856065</v>
       </c>
       <c r="C29" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="12">
       <c r="A30" s="11" t="n">
-        <v>-0.7543858803708186</v>
+        <v>-0.754385880370819</v>
       </c>
       <c r="B30" s="11" t="n">
-        <v>-0.5480934246161641</v>
+        <v>-0.5480934246161639</v>
       </c>
       <c r="C30" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" s="12">
       <c r="A31" s="11" t="n">
-        <v>-0.4662361147021783</v>
+        <v>-0.466236114702178</v>
       </c>
       <c r="B31" s="11" t="n">
-        <v>-0.8075446389876827</v>
+        <v>-0.807544638987683</v>
       </c>
       <c r="C31" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="12">
       <c r="A32" s="11" t="n">
-        <v>-0.09746988917940086</v>
+        <v>-0.0974698891794009</v>
       </c>
       <c r="B32" s="11" t="n">
-        <v>-0.9273640489654993</v>
+        <v>-0.927364048965499</v>
       </c>
       <c r="C32" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="12">
       <c r="A33" s="11" t="n">
-        <v>0.2881497656686403</v>
+        <v>0.28814976566864</v>
       </c>
       <c r="B33" s="11" t="n">
         <v>-0.886833790039282</v>
       </c>
       <c r="C33" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="12">
       <c r="A34" s="11" t="n">
-        <v>0.6239457082741325</v>
+        <v>0.623945708274133</v>
       </c>
       <c r="B34" s="11" t="n">
         <v>-0.692961912183217</v>
       </c>
       <c r="C34" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="12">
       <c r="A35" s="11" t="n">
-        <v>0.8518557695502182</v>
+        <v>0.851855769550218</v>
       </c>
       <c r="B35" s="11" t="n">
-        <v>-0.3792706243493358</v>
+        <v>-0.379270624349336</v>
       </c>
       <c r="C35" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" s="12">
@@ -2853,10 +2854,10 @@
     </row>
     <row r="37" ht="15" customHeight="1" s="12">
       <c r="A37" s="11" t="n">
-        <v>0.9324722294043558</v>
+        <v>0.932472229404356</v>
       </c>
       <c r="B37" s="11" t="n">
-        <v>0.3612416661871529</v>
+        <v>0.361241666187153</v>
       </c>
       <c r="C37" s="11" t="n">
         <v>0</v>
@@ -2864,10 +2865,10 @@
     </row>
     <row r="38" ht="15" customHeight="1" s="12">
       <c r="A38" s="11" t="n">
-        <v>0.7390089172206591</v>
+        <v>0.739008917220659</v>
       </c>
       <c r="B38" s="11" t="n">
-        <v>0.6736956436465572</v>
+        <v>0.673695643646557</v>
       </c>
       <c r="C38" s="11" t="n">
         <v>0</v>
@@ -2875,10 +2876,10 @@
     </row>
     <row r="39" ht="15" customHeight="1" s="12">
       <c r="A39" s="11" t="n">
-        <v>0.4457383557765383</v>
+        <v>0.445738355776538</v>
       </c>
       <c r="B39" s="11" t="n">
-        <v>0.8951632913550623</v>
+        <v>0.895163291355062</v>
       </c>
       <c r="C39" s="11" t="n">
         <v>0</v>
@@ -2886,10 +2887,10 @@
     </row>
     <row r="40" ht="15" customHeight="1" s="12">
       <c r="A40" s="11" t="n">
-        <v>0.09226835946330202</v>
+        <v>0.092268359463302</v>
       </c>
       <c r="B40" s="11" t="n">
-        <v>0.9957341762950345</v>
+        <v>0.995734176295034</v>
       </c>
       <c r="C40" s="11" t="n">
         <v>0</v>
@@ -2897,7 +2898,7 @@
     </row>
     <row r="41" ht="15" customHeight="1" s="12">
       <c r="A41" s="11" t="n">
-        <v>-0.2736629900720829</v>
+        <v>-0.273662990072083</v>
       </c>
       <c r="B41" s="11" t="n">
         <v>0.961825643172819</v>
@@ -2908,10 +2909,10 @@
     </row>
     <row r="42" ht="15" customHeight="1" s="12">
       <c r="A42" s="11" t="n">
-        <v>-0.6026346363792563</v>
+        <v>-0.602634636379256</v>
       </c>
       <c r="B42" s="11" t="n">
-        <v>0.7980172272802396</v>
+        <v>0.79801722728024</v>
       </c>
       <c r="C42" s="11" t="n">
         <v>0</v>
@@ -2919,10 +2920,10 @@
     </row>
     <row r="43" ht="15" customHeight="1" s="12">
       <c r="A43" s="11" t="n">
-        <v>-0.8502171357296142</v>
+        <v>-0.850217135729614</v>
       </c>
       <c r="B43" s="11" t="n">
-        <v>0.5264321628773557</v>
+        <v>0.5264321628773559</v>
       </c>
       <c r="C43" s="11" t="n">
         <v>0</v>
@@ -2930,10 +2931,10 @@
     </row>
     <row r="44" ht="15" customHeight="1" s="12">
       <c r="A44" s="11" t="n">
-        <v>-0.9829730996839018</v>
+        <v>-0.982973099683902</v>
       </c>
       <c r="B44" s="11" t="n">
-        <v>0.1837495178165704</v>
+        <v>0.18374951781657</v>
       </c>
       <c r="C44" s="11" t="n">
         <v>0</v>
@@ -2941,10 +2942,10 @@
     </row>
     <row r="45" ht="15" customHeight="1" s="12">
       <c r="A45" s="11" t="n">
-        <v>-0.9829730996839018</v>
+        <v>-0.982973099683902</v>
       </c>
       <c r="B45" s="11" t="n">
-        <v>-0.1837495178165701</v>
+        <v>-0.18374951781657</v>
       </c>
       <c r="C45" s="11" t="n">
         <v>0</v>
@@ -2952,10 +2953,10 @@
     </row>
     <row r="46" ht="15" customHeight="1" s="12">
       <c r="A46" s="11" t="n">
-        <v>-0.8502171357296141</v>
+        <v>-0.850217135729614</v>
       </c>
       <c r="B46" s="11" t="n">
-        <v>-0.5264321628773558</v>
+        <v>-0.5264321628773559</v>
       </c>
       <c r="C46" s="11" t="n">
         <v>0</v>
@@ -2963,10 +2964,10 @@
     </row>
     <row r="47" ht="15" customHeight="1" s="12">
       <c r="A47" s="11" t="n">
-        <v>-0.6026346363792565</v>
+        <v>-0.602634636379257</v>
       </c>
       <c r="B47" s="11" t="n">
-        <v>-0.7980172272802395</v>
+        <v>-0.798017227280239</v>
       </c>
       <c r="C47" s="11" t="n">
         <v>0</v>
@@ -2974,7 +2975,7 @@
     </row>
     <row r="48" ht="15" customHeight="1" s="12">
       <c r="A48" s="11" t="n">
-        <v>-0.2736629900720831</v>
+        <v>-0.273662990072083</v>
       </c>
       <c r="B48" s="11" t="n">
         <v>-0.961825643172819</v>
@@ -2985,10 +2986,10 @@
     </row>
     <row r="49" ht="15" customHeight="1" s="12">
       <c r="A49" s="11" t="n">
-        <v>0.09226835946330154</v>
+        <v>0.0922683594633016</v>
       </c>
       <c r="B49" s="11" t="n">
-        <v>-0.9957341762950346</v>
+        <v>-0.995734176295035</v>
       </c>
       <c r="C49" s="11" t="n">
         <v>0</v>
@@ -2996,10 +2997,10 @@
     </row>
     <row r="50" ht="15" customHeight="1" s="12">
       <c r="A50" s="11" t="n">
-        <v>0.4457383557765385</v>
+        <v>0.445738355776538</v>
       </c>
       <c r="B50" s="11" t="n">
-        <v>-0.8951632913550622</v>
+        <v>-0.895163291355062</v>
       </c>
       <c r="C50" s="11" t="n">
         <v>0</v>
@@ -3007,10 +3008,10 @@
     </row>
     <row r="51" ht="15" customHeight="1" s="12">
       <c r="A51" s="11" t="n">
-        <v>0.7390089172206592</v>
+        <v>0.739008917220659</v>
       </c>
       <c r="B51" s="11" t="n">
-        <v>-0.6736956436465571</v>
+        <v>-0.673695643646557</v>
       </c>
       <c r="C51" s="11" t="n">
         <v>0</v>
@@ -3018,7 +3019,7 @@
     </row>
     <row r="52" ht="15" customHeight="1" s="12">
       <c r="A52" s="11" t="n">
-        <v>0.9324722294043558</v>
+        <v>0.932472229404356</v>
       </c>
       <c r="B52" s="11" t="n">
         <v>-0.361241666187153</v>
@@ -3029,24 +3030,24 @@
     </row>
     <row r="53" ht="15" customHeight="1" s="12">
       <c r="A53" s="11" t="n">
-        <v>0.9324722294043558</v>
+        <v>0.932472229404356</v>
       </c>
       <c r="B53" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C53" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="12">
       <c r="A54" s="11" t="n">
-        <v>0.8518557695502186</v>
+        <v>0.851855769550219</v>
       </c>
       <c r="B54" s="11" t="n">
-        <v>0.3792706243493351</v>
+        <v>0.379270624349335</v>
       </c>
       <c r="C54" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="12">
@@ -3054,252 +3055,252 @@
         <v>0.623945708274133</v>
       </c>
       <c r="B55" s="11" t="n">
-        <v>0.6929619121832167</v>
+        <v>0.692961912183217</v>
       </c>
       <c r="C55" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="12">
       <c r="A56" s="11" t="n">
-        <v>0.2881497656686405</v>
+        <v>0.28814976566864</v>
       </c>
       <c r="B56" s="11" t="n">
-        <v>0.8868337900392819</v>
+        <v>0.886833790039282</v>
       </c>
       <c r="C56" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" s="12">
       <c r="A57" s="11" t="n">
-        <v>-0.09746988917940001</v>
+        <v>-0.0974698891794</v>
       </c>
       <c r="B57" s="11" t="n">
-        <v>0.9273640489654994</v>
+        <v>0.927364048965499</v>
       </c>
       <c r="C57" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="12">
       <c r="A58" s="11" t="n">
-        <v>-0.4662361147021777</v>
+        <v>-0.466236114702178</v>
       </c>
       <c r="B58" s="11" t="n">
         <v>0.807544638987683</v>
       </c>
       <c r="C58" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" s="12">
       <c r="A59" s="11" t="n">
-        <v>-0.7543858803708183</v>
+        <v>-0.754385880370818</v>
       </c>
       <c r="B59" s="11" t="n">
-        <v>0.5480934246161643</v>
+        <v>0.5480934246161639</v>
       </c>
       <c r="C59" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" s="12">
       <c r="A60" s="11" t="n">
-        <v>-0.9120954739427733</v>
+        <v>-0.912095473942773</v>
       </c>
       <c r="B60" s="11" t="n">
-        <v>0.1938718778560655</v>
+        <v>0.193871877856065</v>
       </c>
       <c r="C60" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="12">
       <c r="A61" s="11" t="n">
-        <v>-0.9120954739427735</v>
+        <v>-0.912095473942773</v>
       </c>
       <c r="B61" s="11" t="n">
-        <v>-0.1938718778560649</v>
+        <v>-0.193871877856065</v>
       </c>
       <c r="C61" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="12">
       <c r="A62" s="11" t="n">
-        <v>-0.7543858803708186</v>
+        <v>-0.754385880370819</v>
       </c>
       <c r="B62" s="11" t="n">
-        <v>-0.5480934246161641</v>
+        <v>-0.5480934246161639</v>
       </c>
       <c r="C62" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" s="12">
       <c r="A63" s="11" t="n">
-        <v>-0.4662361147021783</v>
+        <v>-0.466236114702178</v>
       </c>
       <c r="B63" s="11" t="n">
-        <v>-0.8075446389876827</v>
+        <v>-0.807544638987683</v>
       </c>
       <c r="C63" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" s="12">
       <c r="A64" s="11" t="n">
-        <v>-0.09746988917940086</v>
+        <v>-0.0974698891794009</v>
       </c>
       <c r="B64" s="11" t="n">
-        <v>-0.9273640489654993</v>
+        <v>-0.927364048965499</v>
       </c>
       <c r="C64" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" s="12">
       <c r="A65" s="11" t="n">
-        <v>0.2881497656686403</v>
+        <v>0.28814976566864</v>
       </c>
       <c r="B65" s="11" t="n">
         <v>-0.886833790039282</v>
       </c>
       <c r="C65" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" s="12">
       <c r="A66" s="11" t="n">
-        <v>0.6239457082741325</v>
+        <v>0.623945708274133</v>
       </c>
       <c r="B66" s="11" t="n">
         <v>-0.692961912183217</v>
       </c>
       <c r="C66" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" s="12">
       <c r="A67" s="11" t="n">
-        <v>0.8518557695502182</v>
+        <v>0.851855769550218</v>
       </c>
       <c r="B67" s="11" t="n">
-        <v>-0.3792706243493358</v>
+        <v>-0.379270624349336</v>
       </c>
       <c r="C67" s="11" t="n">
-        <v>-0.3612416661871529</v>
+        <v>-0.361241666187153</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" s="12">
       <c r="A68" s="11" t="n">
-        <v>0.7390089172206591</v>
+        <v>0.739008917220659</v>
       </c>
       <c r="B68" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C68" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1" s="12">
       <c r="A69" s="11" t="n">
-        <v>0.6400004959363221</v>
+        <v>0.640000495936322</v>
       </c>
       <c r="B69" s="11" t="n">
-        <v>0.3695044586103295</v>
+        <v>0.369504458610329</v>
       </c>
       <c r="C69" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1" s="12">
       <c r="A70" s="11" t="n">
-        <v>0.3695044586103296</v>
+        <v>0.36950445861033</v>
       </c>
       <c r="B70" s="11" t="n">
         <v>0.640000495936322</v>
       </c>
       <c r="C70" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1" s="12">
       <c r="A71" s="11" t="n">
-        <v>4.525124525078157e-17</v>
+        <v>4.52512452507816e-17</v>
       </c>
       <c r="B71" s="11" t="n">
-        <v>0.7390089172206591</v>
+        <v>0.739008917220659</v>
       </c>
       <c r="C71" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1" s="12">
       <c r="A72" s="11" t="n">
-        <v>-0.3695044586103294</v>
+        <v>-0.369504458610329</v>
       </c>
       <c r="B72" s="11" t="n">
-        <v>0.6400004959363221</v>
+        <v>0.640000495936322</v>
       </c>
       <c r="C72" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1" s="12">
       <c r="A73" s="11" t="n">
-        <v>-0.6400004959363219</v>
+        <v>-0.640000495936322</v>
       </c>
       <c r="B73" s="11" t="n">
-        <v>0.3695044586103298</v>
+        <v>0.36950445861033</v>
       </c>
       <c r="C73" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1" s="12">
       <c r="A74" s="11" t="n">
-        <v>-0.7390089172206591</v>
+        <v>-0.739008917220659</v>
       </c>
       <c r="B74" s="11" t="n">
-        <v>9.050249050156315e-17</v>
+        <v>9.05024905015632e-17</v>
       </c>
       <c r="C74" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1" s="12">
       <c r="A75" s="11" t="n">
-        <v>-0.6400004959363222</v>
+        <v>-0.640000495936322</v>
       </c>
       <c r="B75" s="11" t="n">
-        <v>-0.3695044586103293</v>
+        <v>-0.369504458610329</v>
       </c>
       <c r="C75" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1" s="12">
       <c r="A76" s="11" t="n">
-        <v>-0.3695044586103299</v>
+        <v>-0.36950445861033</v>
       </c>
       <c r="B76" s="11" t="n">
-        <v>-0.6400004959363219</v>
+        <v>-0.640000495936322</v>
       </c>
       <c r="C76" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1" s="12">
       <c r="A77" s="11" t="n">
-        <v>-1.357537357523447e-16</v>
+        <v>-1.35753735752345e-16</v>
       </c>
       <c r="B77" s="11" t="n">
-        <v>-0.7390089172206591</v>
+        <v>-0.739008917220659</v>
       </c>
       <c r="C77" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1" s="12">
@@ -3307,98 +3308,98 @@
         <v>0.369504458610329</v>
       </c>
       <c r="B78" s="11" t="n">
-        <v>-0.6400004959363224</v>
+        <v>-0.640000495936322</v>
       </c>
       <c r="C78" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1" s="12">
       <c r="A79" s="11" t="n">
-        <v>0.6400004959363219</v>
+        <v>0.640000495936322</v>
       </c>
       <c r="B79" s="11" t="n">
-        <v>-0.3695044586103299</v>
+        <v>-0.36950445861033</v>
       </c>
       <c r="C79" s="11" t="n">
-        <v>-0.6736956436465572</v>
+        <v>-0.673695643646557</v>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1" s="12">
       <c r="A80" s="11" t="n">
-        <v>0.4457383557765383</v>
+        <v>0.445738355776538</v>
       </c>
       <c r="B80" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C80" s="11" t="n">
-        <v>-0.8951632913550623</v>
+        <v>-0.895163291355062</v>
       </c>
     </row>
     <row r="81" ht="15" customHeight="1" s="12">
       <c r="A81" s="11" t="n">
-        <v>0.2779133191239516</v>
+        <v>0.277913319123952</v>
       </c>
       <c r="B81" s="11" t="n">
         <v>0.348492279489633</v>
       </c>
       <c r="C81" s="11" t="n">
-        <v>-0.8951632913550623</v>
+        <v>-0.895163291355062</v>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1" s="12">
       <c r="A82" s="11" t="n">
-        <v>-0.09918611522754722</v>
+        <v>-0.09918611522754719</v>
       </c>
       <c r="B82" s="11" t="n">
-        <v>0.4345627645765794</v>
+        <v>0.434562764576579</v>
       </c>
       <c r="C82" s="11" t="n">
-        <v>-0.8951632913550623</v>
+        <v>-0.895163291355062</v>
       </c>
     </row>
     <row r="83" ht="15" customHeight="1" s="12">
       <c r="A83" s="11" t="n">
-        <v>-0.4015963817846734</v>
+        <v>-0.401596381784673</v>
       </c>
       <c r="B83" s="11" t="n">
-        <v>0.1933986244724369</v>
+        <v>0.193398624472437</v>
       </c>
       <c r="C83" s="11" t="n">
-        <v>-0.8951632913550623</v>
+        <v>-0.895163291355062</v>
       </c>
     </row>
     <row r="84" ht="15" customHeight="1" s="12">
       <c r="A84" s="11" t="n">
-        <v>-0.4015963817846734</v>
+        <v>-0.401596381784673</v>
       </c>
       <c r="B84" s="11" t="n">
-        <v>-0.1933986244724368</v>
+        <v>-0.193398624472437</v>
       </c>
       <c r="C84" s="11" t="n">
-        <v>-0.8951632913550623</v>
+        <v>-0.895163291355062</v>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1" s="12">
       <c r="A85" s="11" t="n">
-        <v>-0.09918611522754733</v>
+        <v>-0.09918611522754731</v>
       </c>
       <c r="B85" s="11" t="n">
-        <v>-0.4345627645765794</v>
+        <v>-0.434562764576579</v>
       </c>
       <c r="C85" s="11" t="n">
-        <v>-0.8951632913550623</v>
+        <v>-0.895163291355062</v>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1" s="12">
       <c r="A86" s="11" t="n">
-        <v>0.2779133191239515</v>
+        <v>0.277913319123951</v>
       </c>
       <c r="B86" s="11" t="n">
-        <v>-0.3484922794896331</v>
+        <v>-0.348492279489633</v>
       </c>
       <c r="C86" s="11" t="n">
-        <v>-0.8951632913550623</v>
+        <v>-0.895163291355062</v>
       </c>
     </row>
     <row r="87" ht="15" customHeight="1" s="12">
@@ -3449,7 +3450,7 @@
     </row>
     <row r="2" ht="15" customHeight="1" s="12">
       <c r="A2" s="11" t="n">
-        <v>0.1736481776669304</v>
+        <v>0.17364817766693</v>
       </c>
       <c r="B2" s="11" t="n">
         <v>0</v>
@@ -3460,10 +3461,10 @@
     </row>
     <row r="3" ht="15" customHeight="1" s="12">
       <c r="A3" s="11" t="n">
-        <v>-0.1736481776669304</v>
+        <v>-0.17364817766693</v>
       </c>
       <c r="B3" s="11" t="n">
-        <v>2.126576849575772e-17</v>
+        <v>2.12657684957577e-17</v>
       </c>
       <c r="C3" s="11" t="n">
         <v>0.984807753012208</v>
@@ -3471,90 +3472,90 @@
     </row>
     <row r="4" ht="15" customHeight="1" s="12">
       <c r="A4" s="11" t="n">
-        <v>0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="B4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="12">
       <c r="A5" s="11" t="n">
-        <v>0.3535533905932738</v>
+        <v>0.353553390593274</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>0.3535533905932738</v>
+        <v>0.353553390593274</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="12">
       <c r="A6" s="11" t="n">
-        <v>3.061616997868384e-17</v>
+        <v>3.06161699786838e-17</v>
       </c>
       <c r="B6" s="11" t="n">
-        <v>0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="12">
       <c r="A7" s="11" t="n">
-        <v>-0.3535533905932738</v>
+        <v>-0.353553390593274</v>
       </c>
       <c r="B7" s="11" t="n">
-        <v>0.3535533905932738</v>
+        <v>0.353553390593274</v>
       </c>
       <c r="C7" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="12">
       <c r="A8" s="11" t="n">
-        <v>-0.5000000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="B8" s="11" t="n">
-        <v>6.123233995736767e-17</v>
+        <v>6.12323399573677e-17</v>
       </c>
       <c r="C8" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="12">
       <c r="A9" s="11" t="n">
-        <v>-0.3535533905932739</v>
+        <v>-0.353553390593274</v>
       </c>
       <c r="B9" s="11" t="n">
-        <v>-0.3535533905932738</v>
+        <v>-0.353553390593274</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="12">
       <c r="A10" s="11" t="n">
-        <v>-9.184850993605151e-17</v>
+        <v>-9.18485099360515e-17</v>
       </c>
       <c r="B10" s="11" t="n">
-        <v>-0.5000000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="C10" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="12">
       <c r="A11" s="11" t="n">
-        <v>0.3535533905932737</v>
+        <v>0.353553390593274</v>
       </c>
       <c r="B11" s="11" t="n">
-        <v>-0.3535533905932739</v>
+        <v>-0.353553390593274</v>
       </c>
       <c r="C11" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="12">
@@ -3565,29 +3566,29 @@
         <v>0</v>
       </c>
       <c r="C12" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="12">
       <c r="A13" s="11" t="n">
-        <v>0.6782986680778567</v>
+        <v>0.678298668077857</v>
       </c>
       <c r="B13" s="11" t="n">
-        <v>0.3559986035327536</v>
+        <v>0.355998603532754</v>
       </c>
       <c r="C13" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="12">
       <c r="A14" s="11" t="n">
-        <v>0.4351628425651916</v>
+        <v>0.435162842565192</v>
       </c>
       <c r="B14" s="11" t="n">
-        <v>0.6304422172444096</v>
+        <v>0.63044221724441</v>
       </c>
       <c r="C14" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="12">
@@ -3595,76 +3596,76 @@
         <v>0.09233645410159939</v>
       </c>
       <c r="B15" s="11" t="n">
-        <v>0.7604591166377114</v>
+        <v>0.760459116637711</v>
       </c>
       <c r="C15" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="12">
       <c r="A16" s="11" t="n">
-        <v>-0.2716431032217672</v>
+        <v>-0.271643103221767</v>
       </c>
       <c r="B16" s="11" t="n">
-        <v>0.7162639969351478</v>
+        <v>0.716263996935148</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="12">
       <c r="A17" s="11" t="n">
-        <v>-0.5733924992513005</v>
+        <v>-0.573392499251301</v>
       </c>
       <c r="B17" s="11" t="n">
-        <v>0.5079814274516465</v>
+        <v>0.507981427451647</v>
       </c>
       <c r="C17" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="12">
       <c r="A18" s="11" t="n">
-        <v>-0.7437845838310684</v>
+        <v>-0.743784583831068</v>
       </c>
       <c r="B18" s="11" t="n">
-        <v>0.1833264347788107</v>
+        <v>0.183326434778811</v>
       </c>
       <c r="C18" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="12">
       <c r="A19" s="11" t="n">
-        <v>-0.7437845838310685</v>
+        <v>-0.743784583831068</v>
       </c>
       <c r="B19" s="11" t="n">
-        <v>-0.1833264347788102</v>
+        <v>-0.18332643477881</v>
       </c>
       <c r="C19" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="12">
       <c r="A20" s="11" t="n">
-        <v>-0.5733924992513009</v>
+        <v>-0.573392499251301</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>-0.5079814274516462</v>
+        <v>-0.507981427451646</v>
       </c>
       <c r="C20" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="12">
       <c r="A21" s="11" t="n">
-        <v>-0.2716431032217675</v>
+        <v>-0.271643103221767</v>
       </c>
       <c r="B21" s="11" t="n">
-        <v>-0.7162639969351478</v>
+        <v>-0.716263996935148</v>
       </c>
       <c r="C21" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="12">
@@ -3672,131 +3673,131 @@
         <v>0.0923364541015987</v>
       </c>
       <c r="B22" s="11" t="n">
-        <v>-0.7604591166377115</v>
+        <v>-0.760459116637712</v>
       </c>
       <c r="C22" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="12">
       <c r="A23" s="11" t="n">
-        <v>0.4351628425651914</v>
+        <v>0.435162842565191</v>
       </c>
       <c r="B23" s="11" t="n">
-        <v>-0.6304422172444099</v>
+        <v>-0.63044221724441</v>
       </c>
       <c r="C23" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="12">
       <c r="A24" s="11" t="n">
-        <v>0.6782986680778564</v>
+        <v>0.678298668077856</v>
       </c>
       <c r="B24" s="11" t="n">
-        <v>-0.3559986035327541</v>
+        <v>-0.355998603532754</v>
       </c>
       <c r="C24" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="12">
       <c r="A25" s="11" t="n">
-        <v>0.9396926207859084</v>
+        <v>0.939692620785908</v>
       </c>
       <c r="B25" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" s="12">
       <c r="A26" s="11" t="n">
-        <v>0.8681627791959909</v>
+        <v>0.8681627791959911</v>
       </c>
       <c r="B26" s="11" t="n">
-        <v>0.3596047974904982</v>
+        <v>0.359604797490498</v>
       </c>
       <c r="C26" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="12">
       <c r="A27" s="11" t="n">
-        <v>0.6644630243886748</v>
+        <v>0.664463024388675</v>
       </c>
       <c r="B27" s="11" t="n">
-        <v>0.6644630243886747</v>
+        <v>0.664463024388675</v>
       </c>
       <c r="C27" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" s="12">
       <c r="A28" s="11" t="n">
-        <v>0.3596047974904982</v>
+        <v>0.359604797490498</v>
       </c>
       <c r="B28" s="11" t="n">
-        <v>0.8681627791959909</v>
+        <v>0.8681627791959911</v>
       </c>
       <c r="C28" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="12">
       <c r="A29" s="11" t="n">
-        <v>5.753957801139251e-17</v>
+        <v>5.75395780113925e-17</v>
       </c>
       <c r="B29" s="11" t="n">
-        <v>0.9396926207859084</v>
+        <v>0.939692620785908</v>
       </c>
       <c r="C29" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="12">
       <c r="A30" s="11" t="n">
-        <v>-0.3596047974904981</v>
+        <v>-0.359604797490498</v>
       </c>
       <c r="B30" s="11" t="n">
-        <v>0.8681627791959909</v>
+        <v>0.8681627791959911</v>
       </c>
       <c r="C30" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" s="12">
       <c r="A31" s="11" t="n">
-        <v>-0.6644630243886747</v>
+        <v>-0.664463024388675</v>
       </c>
       <c r="B31" s="11" t="n">
-        <v>0.6644630243886748</v>
+        <v>0.664463024388675</v>
       </c>
       <c r="C31" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="12">
       <c r="A32" s="11" t="n">
-        <v>-0.8681627791959909</v>
+        <v>-0.8681627791959911</v>
       </c>
       <c r="B32" s="11" t="n">
-        <v>0.3596047974904982</v>
+        <v>0.359604797490498</v>
       </c>
       <c r="C32" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="12">
       <c r="A33" s="11" t="n">
-        <v>-0.9396926207859084</v>
+        <v>-0.939692620785908</v>
       </c>
       <c r="B33" s="11" t="n">
         <v>1.15079156022785e-16</v>
       </c>
       <c r="C33" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="12">
@@ -3804,76 +3805,76 @@
         <v>-0.8681627791959911</v>
       </c>
       <c r="B34" s="11" t="n">
-        <v>-0.3596047974904981</v>
+        <v>-0.359604797490498</v>
       </c>
       <c r="C34" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="12">
       <c r="A35" s="11" t="n">
-        <v>-0.6644630243886749</v>
+        <v>-0.664463024388675</v>
       </c>
       <c r="B35" s="11" t="n">
-        <v>-0.6644630243886747</v>
+        <v>-0.664463024388675</v>
       </c>
       <c r="C35" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" s="12">
       <c r="A36" s="11" t="n">
-        <v>-0.3596047974904987</v>
+        <v>-0.359604797490499</v>
       </c>
       <c r="B36" s="11" t="n">
-        <v>-0.8681627791959907</v>
+        <v>-0.8681627791959911</v>
       </c>
       <c r="C36" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="12">
       <c r="A37" s="11" t="n">
-        <v>-1.726187340341775e-16</v>
+        <v>-1.72618734034178e-16</v>
       </c>
       <c r="B37" s="11" t="n">
-        <v>-0.9396926207859084</v>
+        <v>-0.939692620785908</v>
       </c>
       <c r="C37" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="12">
       <c r="A38" s="11" t="n">
-        <v>0.3596047974904983</v>
+        <v>0.359604797490498</v>
       </c>
       <c r="B38" s="11" t="n">
-        <v>-0.8681627791959908</v>
+        <v>-0.8681627791959911</v>
       </c>
       <c r="C38" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="12">
       <c r="A39" s="11" t="n">
-        <v>0.6644630243886746</v>
+        <v>0.664463024388675</v>
       </c>
       <c r="B39" s="11" t="n">
-        <v>-0.6644630243886749</v>
+        <v>-0.664463024388675</v>
       </c>
       <c r="C39" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="12">
       <c r="A40" s="11" t="n">
-        <v>0.8681627791959907</v>
+        <v>0.8681627791959911</v>
       </c>
       <c r="B40" s="11" t="n">
-        <v>-0.3596047974904987</v>
+        <v>-0.359604797490499</v>
       </c>
       <c r="C40" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="12">
@@ -3889,10 +3890,10 @@
     </row>
     <row r="42" ht="15" customHeight="1" s="12">
       <c r="A42" s="11" t="n">
-        <v>0.9396926207859084</v>
+        <v>0.939692620785908</v>
       </c>
       <c r="B42" s="11" t="n">
-        <v>0.3420201433256687</v>
+        <v>0.342020143325669</v>
       </c>
       <c r="C42" s="11" t="n">
         <v>0</v>
@@ -3903,7 +3904,7 @@
         <v>0.766044443118978</v>
       </c>
       <c r="B43" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
       <c r="C43" s="11" t="n">
         <v>0</v>
@@ -3911,10 +3912,10 @@
     </row>
     <row r="44" ht="15" customHeight="1" s="12">
       <c r="A44" s="11" t="n">
-        <v>0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="B44" s="11" t="n">
-        <v>0.8660254037844386</v>
+        <v>0.866025403784439</v>
       </c>
       <c r="C44" s="11" t="n">
         <v>0</v>
@@ -3922,7 +3923,7 @@
     </row>
     <row r="45" ht="15" customHeight="1" s="12">
       <c r="A45" s="11" t="n">
-        <v>0.1736481776669304</v>
+        <v>0.17364817766693</v>
       </c>
       <c r="B45" s="11" t="n">
         <v>0.984807753012208</v>
@@ -3933,7 +3934,7 @@
     </row>
     <row r="46" ht="15" customHeight="1" s="12">
       <c r="A46" s="11" t="n">
-        <v>-0.1736481776669303</v>
+        <v>-0.17364817766693</v>
       </c>
       <c r="B46" s="11" t="n">
         <v>0.984807753012208</v>
@@ -3944,10 +3945,10 @@
     </row>
     <row r="47" ht="15" customHeight="1" s="12">
       <c r="A47" s="11" t="n">
-        <v>-0.4999999999999998</v>
+        <v>-0.5</v>
       </c>
       <c r="B47" s="11" t="n">
-        <v>0.8660254037844387</v>
+        <v>0.866025403784439</v>
       </c>
       <c r="C47" s="11" t="n">
         <v>0</v>
@@ -3955,10 +3956,10 @@
     </row>
     <row r="48" ht="15" customHeight="1" s="12">
       <c r="A48" s="11" t="n">
-        <v>-0.7660444431189779</v>
+        <v>-0.766044443118978</v>
       </c>
       <c r="B48" s="11" t="n">
-        <v>0.6427876096865395</v>
+        <v>0.642787609686539</v>
       </c>
       <c r="C48" s="11" t="n">
         <v>0</v>
@@ -3966,10 +3967,10 @@
     </row>
     <row r="49" ht="15" customHeight="1" s="12">
       <c r="A49" s="11" t="n">
-        <v>-0.9396926207859083</v>
+        <v>-0.939692620785908</v>
       </c>
       <c r="B49" s="11" t="n">
-        <v>0.3420201433256689</v>
+        <v>0.342020143325669</v>
       </c>
       <c r="C49" s="11" t="n">
         <v>0</v>
@@ -3980,7 +3981,7 @@
         <v>-1</v>
       </c>
       <c r="B50" s="11" t="n">
-        <v>1.224646799147353e-16</v>
+        <v>1.22464679914735e-16</v>
       </c>
       <c r="C50" s="11" t="n">
         <v>0</v>
@@ -3988,10 +3989,10 @@
     </row>
     <row r="51" ht="15" customHeight="1" s="12">
       <c r="A51" s="11" t="n">
-        <v>-0.9396926207859084</v>
+        <v>-0.939692620785908</v>
       </c>
       <c r="B51" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
       <c r="C51" s="11" t="n">
         <v>0</v>
@@ -4002,7 +4003,7 @@
         <v>-0.766044443118978</v>
       </c>
       <c r="B52" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
       <c r="C52" s="11" t="n">
         <v>0</v>
@@ -4010,10 +4011,10 @@
     </row>
     <row r="53" ht="15" customHeight="1" s="12">
       <c r="A53" s="11" t="n">
-        <v>-0.5000000000000004</v>
+        <v>-0.5</v>
       </c>
       <c r="B53" s="11" t="n">
-        <v>-0.8660254037844384</v>
+        <v>-0.866025403784438</v>
       </c>
       <c r="C53" s="11" t="n">
         <v>0</v>
@@ -4021,7 +4022,7 @@
     </row>
     <row r="54" ht="15" customHeight="1" s="12">
       <c r="A54" s="11" t="n">
-        <v>-0.1736481776669303</v>
+        <v>-0.17364817766693</v>
       </c>
       <c r="B54" s="11" t="n">
         <v>-0.984807753012208</v>
@@ -4035,7 +4036,7 @@
         <v>0.17364817766693</v>
       </c>
       <c r="B55" s="11" t="n">
-        <v>-0.9848077530122081</v>
+        <v>-0.984807753012208</v>
       </c>
       <c r="C55" s="11" t="n">
         <v>0</v>
@@ -4043,10 +4044,10 @@
     </row>
     <row r="56" ht="15" customHeight="1" s="12">
       <c r="A56" s="11" t="n">
-        <v>0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="B56" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
       <c r="C56" s="11" t="n">
         <v>0</v>
@@ -4054,10 +4055,10 @@
     </row>
     <row r="57" ht="15" customHeight="1" s="12">
       <c r="A57" s="11" t="n">
-        <v>0.7660444431189778</v>
+        <v>0.766044443118978</v>
       </c>
       <c r="B57" s="11" t="n">
-        <v>-0.6427876096865396</v>
+        <v>-0.64278760968654</v>
       </c>
       <c r="C57" s="11" t="n">
         <v>0</v>
@@ -4065,10 +4066,10 @@
     </row>
     <row r="58" ht="15" customHeight="1" s="12">
       <c r="A58" s="11" t="n">
-        <v>0.9396926207859081</v>
+        <v>0.939692620785908</v>
       </c>
       <c r="B58" s="11" t="n">
-        <v>-0.3420201433256694</v>
+        <v>-0.342020143325669</v>
       </c>
       <c r="C58" s="11" t="n">
         <v>0</v>
@@ -4076,101 +4077,101 @@
     </row>
     <row r="59" ht="15" customHeight="1" s="12">
       <c r="A59" s="11" t="n">
-        <v>0.9396926207859084</v>
+        <v>0.939692620785908</v>
       </c>
       <c r="B59" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C59" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" s="12">
       <c r="A60" s="11" t="n">
-        <v>0.8681627791959909</v>
+        <v>0.8681627791959911</v>
       </c>
       <c r="B60" s="11" t="n">
-        <v>0.3596047974904982</v>
+        <v>0.359604797490498</v>
       </c>
       <c r="C60" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="12">
       <c r="A61" s="11" t="n">
-        <v>0.6644630243886748</v>
+        <v>0.664463024388675</v>
       </c>
       <c r="B61" s="11" t="n">
-        <v>0.6644630243886747</v>
+        <v>0.664463024388675</v>
       </c>
       <c r="C61" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="12">
       <c r="A62" s="11" t="n">
-        <v>0.3596047974904982</v>
+        <v>0.359604797490498</v>
       </c>
       <c r="B62" s="11" t="n">
-        <v>0.8681627791959909</v>
+        <v>0.8681627791959911</v>
       </c>
       <c r="C62" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" s="12">
       <c r="A63" s="11" t="n">
-        <v>5.753957801139251e-17</v>
+        <v>5.75395780113925e-17</v>
       </c>
       <c r="B63" s="11" t="n">
-        <v>0.9396926207859084</v>
+        <v>0.939692620785908</v>
       </c>
       <c r="C63" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" s="12">
       <c r="A64" s="11" t="n">
-        <v>-0.3596047974904981</v>
+        <v>-0.359604797490498</v>
       </c>
       <c r="B64" s="11" t="n">
-        <v>0.8681627791959909</v>
+        <v>0.8681627791959911</v>
       </c>
       <c r="C64" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" s="12">
       <c r="A65" s="11" t="n">
-        <v>-0.6644630243886747</v>
+        <v>-0.664463024388675</v>
       </c>
       <c r="B65" s="11" t="n">
-        <v>0.6644630243886748</v>
+        <v>0.664463024388675</v>
       </c>
       <c r="C65" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" s="12">
       <c r="A66" s="11" t="n">
-        <v>-0.8681627791959909</v>
+        <v>-0.8681627791959911</v>
       </c>
       <c r="B66" s="11" t="n">
-        <v>0.3596047974904982</v>
+        <v>0.359604797490498</v>
       </c>
       <c r="C66" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" s="12">
       <c r="A67" s="11" t="n">
-        <v>-0.9396926207859084</v>
+        <v>-0.939692620785908</v>
       </c>
       <c r="B67" s="11" t="n">
         <v>1.15079156022785e-16</v>
       </c>
       <c r="C67" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" s="12">
@@ -4178,76 +4179,76 @@
         <v>-0.8681627791959911</v>
       </c>
       <c r="B68" s="11" t="n">
-        <v>-0.3596047974904981</v>
+        <v>-0.359604797490498</v>
       </c>
       <c r="C68" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1" s="12">
       <c r="A69" s="11" t="n">
-        <v>-0.6644630243886749</v>
+        <v>-0.664463024388675</v>
       </c>
       <c r="B69" s="11" t="n">
-        <v>-0.6644630243886747</v>
+        <v>-0.664463024388675</v>
       </c>
       <c r="C69" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1" s="12">
       <c r="A70" s="11" t="n">
-        <v>-0.3596047974904987</v>
+        <v>-0.359604797490499</v>
       </c>
       <c r="B70" s="11" t="n">
-        <v>-0.8681627791959907</v>
+        <v>-0.8681627791959911</v>
       </c>
       <c r="C70" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1" s="12">
       <c r="A71" s="11" t="n">
-        <v>-1.726187340341775e-16</v>
+        <v>-1.72618734034178e-16</v>
       </c>
       <c r="B71" s="11" t="n">
-        <v>-0.9396926207859084</v>
+        <v>-0.939692620785908</v>
       </c>
       <c r="C71" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1" s="12">
       <c r="A72" s="11" t="n">
-        <v>0.3596047974904983</v>
+        <v>0.359604797490498</v>
       </c>
       <c r="B72" s="11" t="n">
-        <v>-0.8681627791959908</v>
+        <v>-0.8681627791959911</v>
       </c>
       <c r="C72" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1" s="12">
       <c r="A73" s="11" t="n">
-        <v>0.6644630243886746</v>
+        <v>0.664463024388675</v>
       </c>
       <c r="B73" s="11" t="n">
-        <v>-0.6644630243886749</v>
+        <v>-0.664463024388675</v>
       </c>
       <c r="C73" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1" s="12">
       <c r="A74" s="11" t="n">
-        <v>0.8681627791959907</v>
+        <v>0.8681627791959911</v>
       </c>
       <c r="B74" s="11" t="n">
-        <v>-0.3596047974904987</v>
+        <v>-0.359604797490499</v>
       </c>
       <c r="C74" s="11" t="n">
-        <v>-0.3420201433256687</v>
+        <v>-0.342020143325669</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1" s="12">
@@ -4258,29 +4259,29 @@
         <v>0</v>
       </c>
       <c r="C75" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1" s="12">
       <c r="A76" s="11" t="n">
-        <v>0.6782986680778567</v>
+        <v>0.678298668077857</v>
       </c>
       <c r="B76" s="11" t="n">
-        <v>0.3559986035327536</v>
+        <v>0.355998603532754</v>
       </c>
       <c r="C76" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1" s="12">
       <c r="A77" s="11" t="n">
-        <v>0.4351628425651916</v>
+        <v>0.435162842565192</v>
       </c>
       <c r="B77" s="11" t="n">
-        <v>0.6304422172444096</v>
+        <v>0.63044221724441</v>
       </c>
       <c r="C77" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1" s="12">
@@ -4288,76 +4289,76 @@
         <v>0.09233645410159939</v>
       </c>
       <c r="B78" s="11" t="n">
-        <v>0.7604591166377114</v>
+        <v>0.760459116637711</v>
       </c>
       <c r="C78" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1" s="12">
       <c r="A79" s="11" t="n">
-        <v>-0.2716431032217672</v>
+        <v>-0.271643103221767</v>
       </c>
       <c r="B79" s="11" t="n">
-        <v>0.7162639969351478</v>
+        <v>0.716263996935148</v>
       </c>
       <c r="C79" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1" s="12">
       <c r="A80" s="11" t="n">
-        <v>-0.5733924992513005</v>
+        <v>-0.573392499251301</v>
       </c>
       <c r="B80" s="11" t="n">
-        <v>0.5079814274516465</v>
+        <v>0.507981427451647</v>
       </c>
       <c r="C80" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="81" ht="15" customHeight="1" s="12">
       <c r="A81" s="11" t="n">
-        <v>-0.7437845838310684</v>
+        <v>-0.743784583831068</v>
       </c>
       <c r="B81" s="11" t="n">
-        <v>0.1833264347788107</v>
+        <v>0.183326434778811</v>
       </c>
       <c r="C81" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1" s="12">
       <c r="A82" s="11" t="n">
-        <v>-0.7437845838310685</v>
+        <v>-0.743784583831068</v>
       </c>
       <c r="B82" s="11" t="n">
-        <v>-0.1833264347788102</v>
+        <v>-0.18332643477881</v>
       </c>
       <c r="C82" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="83" ht="15" customHeight="1" s="12">
       <c r="A83" s="11" t="n">
-        <v>-0.5733924992513009</v>
+        <v>-0.573392499251301</v>
       </c>
       <c r="B83" s="11" t="n">
-        <v>-0.5079814274516462</v>
+        <v>-0.507981427451646</v>
       </c>
       <c r="C83" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="84" ht="15" customHeight="1" s="12">
       <c r="A84" s="11" t="n">
-        <v>-0.2716431032217675</v>
+        <v>-0.271643103221767</v>
       </c>
       <c r="B84" s="11" t="n">
-        <v>-0.7162639969351478</v>
+        <v>-0.716263996935148</v>
       </c>
       <c r="C84" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1" s="12">
@@ -4365,125 +4366,125 @@
         <v>0.0923364541015987</v>
       </c>
       <c r="B85" s="11" t="n">
-        <v>-0.7604591166377115</v>
+        <v>-0.760459116637712</v>
       </c>
       <c r="C85" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1" s="12">
       <c r="A86" s="11" t="n">
-        <v>0.4351628425651914</v>
+        <v>0.435162842565191</v>
       </c>
       <c r="B86" s="11" t="n">
-        <v>-0.6304422172444099</v>
+        <v>-0.63044221724441</v>
       </c>
       <c r="C86" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="87" ht="15" customHeight="1" s="12">
       <c r="A87" s="11" t="n">
-        <v>0.6782986680778564</v>
+        <v>0.678298668077856</v>
       </c>
       <c r="B87" s="11" t="n">
-        <v>-0.3559986035327541</v>
+        <v>-0.355998603532754</v>
       </c>
       <c r="C87" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1" s="12">
       <c r="A88" s="11" t="n">
-        <v>0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="B88" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C88" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="89" ht="15" customHeight="1" s="12">
       <c r="A89" s="11" t="n">
-        <v>0.3535533905932738</v>
+        <v>0.353553390593274</v>
       </c>
       <c r="B89" s="11" t="n">
-        <v>0.3535533905932738</v>
+        <v>0.353553390593274</v>
       </c>
       <c r="C89" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="90" ht="15" customHeight="1" s="12">
       <c r="A90" s="11" t="n">
-        <v>3.061616997868384e-17</v>
+        <v>3.06161699786838e-17</v>
       </c>
       <c r="B90" s="11" t="n">
-        <v>0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="C90" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="91" ht="15" customHeight="1" s="12">
       <c r="A91" s="11" t="n">
-        <v>-0.3535533905932738</v>
+        <v>-0.353553390593274</v>
       </c>
       <c r="B91" s="11" t="n">
-        <v>0.3535533905932738</v>
+        <v>0.353553390593274</v>
       </c>
       <c r="C91" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="92" ht="15" customHeight="1" s="12">
       <c r="A92" s="11" t="n">
-        <v>-0.5000000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="B92" s="11" t="n">
-        <v>6.123233995736767e-17</v>
+        <v>6.12323399573677e-17</v>
       </c>
       <c r="C92" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="93" ht="15" customHeight="1" s="12">
       <c r="A93" s="11" t="n">
-        <v>-0.3535533905932739</v>
+        <v>-0.353553390593274</v>
       </c>
       <c r="B93" s="11" t="n">
-        <v>-0.3535533905932738</v>
+        <v>-0.353553390593274</v>
       </c>
       <c r="C93" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="94" ht="15" customHeight="1" s="12">
       <c r="A94" s="11" t="n">
-        <v>-9.184850993605151e-17</v>
+        <v>-9.18485099360515e-17</v>
       </c>
       <c r="B94" s="11" t="n">
-        <v>-0.5000000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="C94" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="95" ht="15" customHeight="1" s="12">
       <c r="A95" s="11" t="n">
-        <v>0.3535533905932737</v>
+        <v>0.353553390593274</v>
       </c>
       <c r="B95" s="11" t="n">
-        <v>-0.3535533905932739</v>
+        <v>-0.353553390593274</v>
       </c>
       <c r="C95" s="11" t="n">
-        <v>-0.8660254037844386</v>
+        <v>-0.866025403784439</v>
       </c>
     </row>
     <row r="96" ht="15" customHeight="1" s="12">
       <c r="A96" s="11" t="n">
-        <v>0.1736481776669304</v>
+        <v>0.17364817766693</v>
       </c>
       <c r="B96" s="11" t="n">
         <v>0</v>
@@ -4494,10 +4495,10 @@
     </row>
     <row r="97" ht="15" customHeight="1" s="12">
       <c r="A97" s="11" t="n">
-        <v>-0.1736481776669304</v>
+        <v>-0.17364817766693</v>
       </c>
       <c r="B97" s="11" t="n">
-        <v>2.126576849575772e-17</v>
+        <v>2.12657684957577e-17</v>
       </c>
       <c r="C97" s="11" t="n">
         <v>-0.984807753012208</v>
@@ -12193,8 +12194,8 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -12257,7 +12258,7 @@
         </is>
       </c>
       <c r="C3" s="14" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" ht="52.2" customHeight="1" s="12">
@@ -12287,7 +12288,7 @@
         </is>
       </c>
       <c r="C5" s="14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" ht="51.6" customHeight="1" s="12">
@@ -12302,7 +12303,7 @@
         </is>
       </c>
       <c r="C6" s="14" t="n">
-        <v>1536</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" ht="72.59999999999999" customHeight="1" s="12">
@@ -12317,7 +12318,7 @@
         </is>
       </c>
       <c r="C7" s="14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" ht="28.8" customHeight="1" s="12">
@@ -12398,7 +12399,7 @@
         </is>
       </c>
       <c r="C12" s="14" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" ht="28.8" customHeight="1" s="12">
@@ -12428,7 +12429,7 @@
         </is>
       </c>
       <c r="C14" s="14" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" ht="43.2" customHeight="1" s="12">
@@ -12444,7 +12445,7 @@
       </c>
       <c r="C15" s="14" t="inlineStr">
         <is>
-          <t>LOSOffCentre</t>
+          <t>MultiRefOffCentre</t>
         </is>
       </c>
     </row>
@@ -12505,13 +12506,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" ht="23.85" customHeight="1" s="12">
-      <c r="A20" s="13" t="inlineStr">
+    <row r="20" ht="13.8" customHeight="1" s="12">
+      <c r="A20" s="11" t="inlineStr">
         <is>
-          <t>Calculate the residuals Yes/No</t>
+          <t>Residual On or Off</t>
         </is>
       </c>
-      <c r="B20" s="14" t="inlineStr">
+      <c r="B20" s="13" t="inlineStr">
         <is>
           <t>ResOn</t>
         </is>
@@ -12520,10 +12521,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" ht="57.45" customHeight="1" s="12">
+    <row r="21" ht="35.05" customHeight="1" s="12">
       <c r="A21" s="13" t="inlineStr">
         <is>
-          <t>The maximum number of objects a single ray could go through in one direction.</t>
+          <t>The maximum number of intersection</t>
         </is>
       </c>
       <c r="B21" s="14" t="inlineStr">
@@ -12532,7 +12533,7 @@
         </is>
       </c>
       <c r="C21" s="14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -22107,6 +22108,267 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="n">
+        <v>0.766044443118978</v>
+      </c>
+      <c r="B2" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="n">
+        <v>0.3830222215594891</v>
+      </c>
+      <c r="B3" s="11" t="n">
+        <v>0.6634139481689384</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="n">
+        <v>-0.3830222215594888</v>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>0.6634139481689384</v>
+      </c>
+      <c r="C4" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="n">
+        <v>-0.766044443118978</v>
+      </c>
+      <c r="B5" s="11" t="n">
+        <v>9.381338752702731e-17</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="n">
+        <v>-0.3830222215594893</v>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>-0.6634139481689382</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="11" t="n">
+        <v>0.3830222215594885</v>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>-0.6634139481689387</v>
+      </c>
+      <c r="C7" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="n">
+        <v>0.7071067811865476</v>
+      </c>
+      <c r="B9" s="11" t="n">
+        <v>0.7071067811865475</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="n">
+        <v>6.123233995736766e-17</v>
+      </c>
+      <c r="B10" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="n">
+        <v>-0.7071067811865475</v>
+      </c>
+      <c r="B11" s="11" t="n">
+        <v>0.7071067811865476</v>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="B12" s="11" t="n">
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="11" t="n">
+        <v>-0.7071067811865477</v>
+      </c>
+      <c r="B13" s="11" t="n">
+        <v>-0.7071067811865475</v>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="11" t="n">
+        <v>-1.83697019872103e-16</v>
+      </c>
+      <c r="B14" s="11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C14" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="11" t="n">
+        <v>0.7071067811865474</v>
+      </c>
+      <c r="B15" s="11" t="n">
+        <v>-0.7071067811865477</v>
+      </c>
+      <c r="C15" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="11" t="n">
+        <v>0.766044443118978</v>
+      </c>
+      <c r="B16" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="11" t="n">
+        <v>0.3830222215594891</v>
+      </c>
+      <c r="B17" s="11" t="n">
+        <v>0.6634139481689384</v>
+      </c>
+      <c r="C17" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="n">
+        <v>-0.3830222215594888</v>
+      </c>
+      <c r="B18" s="11" t="n">
+        <v>0.6634139481689384</v>
+      </c>
+      <c r="C18" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="n">
+        <v>-0.766044443118978</v>
+      </c>
+      <c r="B19" s="11" t="n">
+        <v>9.381338752702731e-17</v>
+      </c>
+      <c r="C19" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="n">
+        <v>-0.3830222215594893</v>
+      </c>
+      <c r="B20" s="11" t="n">
+        <v>-0.6634139481689382</v>
+      </c>
+      <c r="C20" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="11" t="n">
+        <v>0.3830222215594885</v>
+      </c>
+      <c r="B21" s="11" t="n">
+        <v>-0.6634139481689387</v>
+      </c>
+      <c r="C21" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B22" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="11" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
@@ -22116,7 +22378,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -22182,13 +22444,13 @@
         <v>299792458</v>
       </c>
       <c r="D2" s="11" t="n">
-        <v>1753008700.7031</v>
+        <v>2400000000</v>
       </c>
       <c r="E2" s="11" t="n">
-        <v>8981.618090872591</v>
+        <v>24.01661485426695</v>
       </c>
       <c r="F2" s="11" t="n">
-        <v>0.0006995605072057964</v>
+        <v>0.2616182732373407</v>
       </c>
       <c r="G2" s="11" t="n">
         <v>1</v>
@@ -22217,10 +22479,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -22277,7 +22539,7 @@
       </c>
       <c r="E2" s="11" t="inlineStr">
         <is>
-          <t>(0.8855548599197771+0.005952846860713298j)</t>
+          <t>(0.8855885559191065+0.003942667577037837j)</t>
         </is>
       </c>
       <c r="F2" s="11" t="inlineStr">
@@ -22311,13 +22573,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="14.4" customHeight="1" s="12">
-      <c r="E7" s="11" t="inlineStr">
-        <is>
-          <t>(0.8855548599197771+0.005952846860713298j)</t>
-        </is>
-      </c>
-    </row>
+    <row r="5" ht="13.8" customHeight="1" s="12"/>
     <row r="14" ht="13.8" customHeight="1" s="12"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -22487,7 +22743,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -22758,7 +23014,7 @@
     <row r="1" ht="15" customHeight="1" s="12">
       <c r="A1" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundar0</t>
+          <t>OuterBoundar000</t>
         </is>
       </c>
       <c r="B1" s="11" t="n">
@@ -22796,7 +23052,7 @@
     <row r="4" ht="15" customHeight="1" s="12">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundar1</t>
+          <t>OuterBoundar001</t>
         </is>
       </c>
       <c r="B4" s="11" t="n">
@@ -22834,7 +23090,7 @@
     <row r="7" ht="15" customHeight="1" s="12">
       <c r="A7" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundar2</t>
+          <t>OuterBoundar002</t>
         </is>
       </c>
       <c r="B7" s="11" t="n">
@@ -22872,7 +23128,7 @@
     <row r="10" ht="15" customHeight="1" s="12">
       <c r="A10" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundar3</t>
+          <t>OuterBoundar003</t>
         </is>
       </c>
       <c r="B10" s="11" t="n">
@@ -22910,7 +23166,7 @@
     <row r="13" ht="15" customHeight="1" s="12">
       <c r="A13" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundar4</t>
+          <t>OuterBoundar004</t>
         </is>
       </c>
       <c r="B13" s="11" t="n">
@@ -22948,7 +23204,7 @@
     <row r="16" ht="15" customHeight="1" s="12">
       <c r="A16" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundar5</t>
+          <t>OuterBoundar005</t>
         </is>
       </c>
       <c r="B16" s="11" t="n">
@@ -22986,7 +23242,7 @@
     <row r="19" ht="15" customHeight="1" s="12">
       <c r="A19" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundar6</t>
+          <t>OuterBoundar006</t>
         </is>
       </c>
       <c r="B19" s="11" t="n">
@@ -23024,7 +23280,7 @@
     <row r="22" ht="15" customHeight="1" s="12">
       <c r="A22" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundar7</t>
+          <t>OuterBoundar007</t>
         </is>
       </c>
       <c r="B22" s="11" t="n">
@@ -23062,7 +23318,7 @@
     <row r="25" ht="15" customHeight="1" s="12">
       <c r="A25" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundar8</t>
+          <t>OuterBoundar008</t>
         </is>
       </c>
       <c r="B25" s="11" t="n">
@@ -23100,7 +23356,7 @@
     <row r="28" ht="15" customHeight="1" s="12">
       <c r="A28" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundar9</t>
+          <t>OuterBoundar009</t>
         </is>
       </c>
       <c r="B28" s="11" t="n">
@@ -23138,7 +23394,7 @@
     <row r="31" ht="15" customHeight="1" s="12">
       <c r="A31" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundar10</t>
+          <t>OuterBoundar010</t>
         </is>
       </c>
       <c r="B31" s="11" t="n">
@@ -23176,7 +23432,7 @@
     <row r="34" ht="15" customHeight="1" s="12">
       <c r="A34" s="11" t="inlineStr">
         <is>
-          <t>Obstacle11</t>
+          <t>Obstacle011</t>
         </is>
       </c>
       <c r="B34" s="11" t="n">

</xml_diff>

<commit_message>
Fixed transmitter check so that it verifies whether the transmitter location being tested is inside an object.
</commit_message>
<xml_diff>
--- a/ParameterIndependent/InputSheet.xlsx
+++ b/ParameterIndependent/InputSheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AngleSpacing" sheetId="1" state="visible" r:id="rId1"/>
@@ -12194,8 +12194,8 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -12318,7 +12318,7 @@
         </is>
       </c>
       <c r="C7" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" ht="28.8" customHeight="1" s="12">
@@ -12445,7 +12445,7 @@
       </c>
       <c r="C15" s="14" t="inlineStr">
         <is>
-          <t>MultiRefOffCentre</t>
+          <t>LOSMovedBox</t>
         </is>
       </c>
     </row>
@@ -22110,19 +22110,22 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="8.67" customWidth="1" style="11" min="1" max="1025"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15" customHeight="1" s="12">
       <c r="A1" s="11" t="n">
         <v>0</v>
       </c>
@@ -22133,7 +22136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15" customHeight="1" s="12">
       <c r="A2" s="11" t="n">
         <v>0.766044443118978</v>
       </c>
@@ -22144,7 +22147,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15" customHeight="1" s="12">
       <c r="A3" s="11" t="n">
         <v>0.3830222215594891</v>
       </c>
@@ -22155,7 +22158,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15" customHeight="1" s="12">
       <c r="A4" s="11" t="n">
         <v>-0.3830222215594888</v>
       </c>
@@ -22166,7 +22169,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15" customHeight="1" s="12">
       <c r="A5" s="11" t="n">
         <v>-0.766044443118978</v>
       </c>
@@ -22177,7 +22180,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15" customHeight="1" s="12">
       <c r="A6" s="11" t="n">
         <v>-0.3830222215594893</v>
       </c>
@@ -22188,7 +22191,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="15" customHeight="1" s="12">
       <c r="A7" s="11" t="n">
         <v>0.3830222215594885</v>
       </c>
@@ -22199,7 +22202,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="15" customHeight="1" s="12">
       <c r="A8" s="11" t="n">
         <v>1</v>
       </c>
@@ -22210,7 +22213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="15" customHeight="1" s="12">
       <c r="A9" s="11" t="n">
         <v>0.7071067811865476</v>
       </c>
@@ -22221,7 +22224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="15" customHeight="1" s="12">
       <c r="A10" s="11" t="n">
         <v>6.123233995736766e-17</v>
       </c>
@@ -22232,7 +22235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="15" customHeight="1" s="12">
       <c r="A11" s="11" t="n">
         <v>-0.7071067811865475</v>
       </c>
@@ -22243,7 +22246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="15" customHeight="1" s="12">
       <c r="A12" s="11" t="n">
         <v>-1</v>
       </c>
@@ -22254,7 +22257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="15" customHeight="1" s="12">
       <c r="A13" s="11" t="n">
         <v>-0.7071067811865477</v>
       </c>
@@ -22265,7 +22268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="15" customHeight="1" s="12">
       <c r="A14" s="11" t="n">
         <v>-1.83697019872103e-16</v>
       </c>
@@ -22276,7 +22279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" ht="15" customHeight="1" s="12">
       <c r="A15" s="11" t="n">
         <v>0.7071067811865474</v>
       </c>
@@ -22287,7 +22290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="15" customHeight="1" s="12">
       <c r="A16" s="11" t="n">
         <v>0.766044443118978</v>
       </c>
@@ -22298,7 +22301,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" ht="15" customHeight="1" s="12">
       <c r="A17" s="11" t="n">
         <v>0.3830222215594891</v>
       </c>
@@ -22309,7 +22312,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" ht="15" customHeight="1" s="12">
       <c r="A18" s="11" t="n">
         <v>-0.3830222215594888</v>
       </c>
@@ -22320,7 +22323,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="15" customHeight="1" s="12">
       <c r="A19" s="11" t="n">
         <v>-0.766044443118978</v>
       </c>
@@ -22331,7 +22334,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" ht="15" customHeight="1" s="12">
       <c r="A20" s="11" t="n">
         <v>-0.3830222215594893</v>
       </c>
@@ -22342,7 +22345,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" ht="15" customHeight="1" s="12">
       <c r="A21" s="11" t="n">
         <v>0.3830222215594885</v>
       </c>
@@ -22353,7 +22356,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" ht="15" customHeight="1" s="12">
       <c r="A22" s="11" t="n">
         <v>0</v>
       </c>
@@ -22365,7 +22368,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
@@ -22569,7 +22574,7 @@
       </c>
       <c r="E3" s="11" t="inlineStr">
         <is>
-          <t>(0.8855548599197771+0.005952846860713298j)</t>
+          <t>(0.8855885559191065+0.003942667577037837j)</t>
         </is>
       </c>
     </row>
@@ -22590,8 +22595,8 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -22709,16 +22714,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="F2" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G2" s="11" t="n">
         <v>0.45</v>
       </c>
-      <c r="G2" s="11" t="n">
-        <v>0</v>
-      </c>
       <c r="H2" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="I2" s="11" t="n">
         <v>0</v>
@@ -23436,10 +23441,10 @@
         </is>
       </c>
       <c r="B34" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C34" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D34" s="11" t="n">
         <v>0</v>
@@ -23447,10 +23452,10 @@
     </row>
     <row r="35" ht="15" customHeight="1" s="12">
       <c r="B35" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C35" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D35" s="11" t="n">
         <v>0</v>
@@ -23458,10 +23463,10 @@
     </row>
     <row r="36" ht="15" customHeight="1" s="12">
       <c r="B36" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C36" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D36" s="11" t="n">
         <v>0.45</v>
@@ -23470,14 +23475,14 @@
     <row r="37" ht="15" customHeight="1" s="12">
       <c r="A37" s="11" t="inlineStr">
         <is>
-          <t>Obstacle12</t>
+          <t>Obstacle012</t>
         </is>
       </c>
       <c r="B37" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C37" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D37" s="11" t="n">
         <v>0</v>
@@ -23485,10 +23490,10 @@
     </row>
     <row r="38" ht="15" customHeight="1" s="12">
       <c r="B38" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C38" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C38" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D38" s="11" t="n">
         <v>0</v>
@@ -23496,10 +23501,10 @@
     </row>
     <row r="39" ht="15" customHeight="1" s="12">
       <c r="B39" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C39" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D39" s="11" t="n">
         <v>0.45</v>
@@ -23508,14 +23513,14 @@
     <row r="40" ht="15" customHeight="1" s="12">
       <c r="A40" s="11" t="inlineStr">
         <is>
-          <t>Obstacle13</t>
+          <t>Obstacle013</t>
         </is>
       </c>
       <c r="B40" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C40" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D40" s="11" t="n">
         <v>0.45</v>
@@ -23523,10 +23528,10 @@
     </row>
     <row r="41" ht="15" customHeight="1" s="12">
       <c r="B41" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C41" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C41" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D41" s="11" t="n">
         <v>0.45</v>
@@ -23534,10 +23539,10 @@
     </row>
     <row r="42" ht="15" customHeight="1" s="12">
       <c r="B42" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C42" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C42" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D42" s="11" t="n">
         <v>0</v>
@@ -23546,14 +23551,14 @@
     <row r="43" ht="15" customHeight="1" s="12">
       <c r="A43" s="11" t="inlineStr">
         <is>
-          <t>Obstacle14</t>
+          <t>Obstacle014</t>
         </is>
       </c>
       <c r="B43" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C43" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D43" s="11" t="n">
         <v>0</v>
@@ -23561,10 +23566,10 @@
     </row>
     <row r="44" ht="15" customHeight="1" s="12">
       <c r="B44" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C44" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D44" s="11" t="n">
         <v>0</v>
@@ -23572,10 +23577,10 @@
     </row>
     <row r="45" ht="15" customHeight="1" s="12">
       <c r="B45" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C45" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D45" s="11" t="n">
         <v>0.45</v>
@@ -23584,14 +23589,14 @@
     <row r="46" ht="15" customHeight="1" s="12">
       <c r="A46" s="11" t="inlineStr">
         <is>
-          <t>Obstacle15</t>
+          <t>Obstacle015</t>
         </is>
       </c>
       <c r="B46" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C46" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D46" s="11" t="n">
         <v>0.45</v>
@@ -23599,10 +23604,10 @@
     </row>
     <row r="47" ht="15" customHeight="1" s="12">
       <c r="B47" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C47" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D47" s="11" t="n">
         <v>0</v>
@@ -23610,10 +23615,10 @@
     </row>
     <row r="48" ht="15" customHeight="1" s="12">
       <c r="B48" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C48" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D48" s="11" t="n">
         <v>0.45</v>
@@ -23622,14 +23627,14 @@
     <row r="49" ht="15" customHeight="1" s="12">
       <c r="A49" s="11" t="inlineStr">
         <is>
-          <t>Obstacle16</t>
+          <t>Obstacle016</t>
         </is>
       </c>
       <c r="B49" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C49" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D49" s="11" t="n">
         <v>0</v>
@@ -23637,10 +23642,10 @@
     </row>
     <row r="50" ht="15" customHeight="1" s="12">
       <c r="B50" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C50" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D50" s="11" t="n">
         <v>0</v>
@@ -23648,10 +23653,10 @@
     </row>
     <row r="51" ht="15" customHeight="1" s="12">
       <c r="B51" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C51" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D51" s="11" t="n">
         <v>0</v>
@@ -23660,14 +23665,14 @@
     <row r="52" ht="15" customHeight="1" s="12">
       <c r="A52" s="11" t="inlineStr">
         <is>
-          <t>Obstacle17</t>
+          <t>Obstacle017</t>
         </is>
       </c>
       <c r="B52" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C52" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D52" s="11" t="n">
         <v>0</v>
@@ -23675,10 +23680,10 @@
     </row>
     <row r="53" ht="15" customHeight="1" s="12">
       <c r="B53" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C53" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D53" s="11" t="n">
         <v>0</v>
@@ -23686,10 +23691,10 @@
     </row>
     <row r="54" ht="15" customHeight="1" s="12">
       <c r="B54" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C54" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C54" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D54" s="11" t="n">
         <v>0</v>
@@ -23698,14 +23703,14 @@
     <row r="55" ht="15" customHeight="1" s="12">
       <c r="A55" s="11" t="inlineStr">
         <is>
-          <t>Obstacle18</t>
+          <t>Obstacle018</t>
         </is>
       </c>
       <c r="B55" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C55" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D55" s="11" t="n">
         <v>0.45</v>
@@ -23713,10 +23718,10 @@
     </row>
     <row r="56" ht="15" customHeight="1" s="12">
       <c r="B56" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C56" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D56" s="11" t="n">
         <v>0.45</v>
@@ -23724,10 +23729,10 @@
     </row>
     <row r="57" ht="15" customHeight="1" s="12">
       <c r="B57" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C57" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C57" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D57" s="11" t="n">
         <v>0.45</v>
@@ -23736,14 +23741,14 @@
     <row r="58" ht="15" customHeight="1" s="12">
       <c r="A58" s="11" t="inlineStr">
         <is>
-          <t>Obstacle19</t>
+          <t>Obstacle019</t>
         </is>
       </c>
       <c r="B58" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C58" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D58" s="11" t="n">
         <v>0.45</v>
@@ -23751,10 +23756,10 @@
     </row>
     <row r="59" ht="15" customHeight="1" s="12">
       <c r="B59" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C59" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D59" s="11" t="n">
         <v>0.45</v>
@@ -23762,10 +23767,10 @@
     </row>
     <row r="60" ht="15" customHeight="1" s="12">
       <c r="B60" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C60" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D60" s="11" t="n">
         <v>0.45</v>
@@ -23774,14 +23779,14 @@
     <row r="61" ht="15" customHeight="1" s="12">
       <c r="A61" s="11" t="inlineStr">
         <is>
-          <t>Obstacle20</t>
+          <t>Obstacle020</t>
         </is>
       </c>
       <c r="B61" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C61" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C61" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D61" s="11" t="n">
         <v>0.45</v>
@@ -23789,10 +23794,10 @@
     </row>
     <row r="62" ht="15" customHeight="1" s="12">
       <c r="B62" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C62" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D62" s="11" t="n">
         <v>0.45</v>
@@ -23800,10 +23805,10 @@
     </row>
     <row r="63" ht="15" customHeight="1" s="12">
       <c r="B63" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C63" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D63" s="11" t="n">
         <v>0</v>
@@ -23812,14 +23817,14 @@
     <row r="64" ht="15" customHeight="1" s="12">
       <c r="A64" s="11" t="inlineStr">
         <is>
-          <t>Obstacle21</t>
+          <t>Obstacle021</t>
         </is>
       </c>
       <c r="B64" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C64" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C64" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D64" s="11" t="n">
         <v>0.45</v>
@@ -23827,10 +23832,10 @@
     </row>
     <row r="65" ht="15" customHeight="1" s="12">
       <c r="B65" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C65" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C65" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D65" s="11" t="n">
         <v>0</v>
@@ -23838,10 +23843,10 @@
     </row>
     <row r="66" ht="15" customHeight="1" s="12">
       <c r="B66" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C66" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D66" s="11" t="n">
         <v>0</v>
@@ -23850,14 +23855,14 @@
     <row r="67" ht="15" customHeight="1" s="12">
       <c r="A67" s="11" t="inlineStr">
         <is>
-          <t>Obstacle22</t>
+          <t>Obstacle022</t>
         </is>
       </c>
       <c r="B67" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C67" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D67" s="11" t="n">
         <v>0</v>
@@ -23865,10 +23870,10 @@
     </row>
     <row r="68" ht="15" customHeight="1" s="12">
       <c r="B68" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C68" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D68" s="11" t="n">
         <v>0.45</v>
@@ -23876,10 +23881,10 @@
     </row>
     <row r="69" ht="15" customHeight="1" s="12">
       <c r="B69" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C69" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D69" s="11" t="n">
         <v>0.45</v>

</xml_diff>

<commit_message>
Room with transmitter location check
</commit_message>
<xml_diff>
--- a/ParameterIndependent/InputSheet.xlsx
+++ b/ParameterIndependent/InputSheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AngleSpacing" sheetId="1" state="visible" r:id="rId1"/>
@@ -12194,8 +12194,8 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -12318,7 +12318,7 @@
         </is>
       </c>
       <c r="C7" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" ht="28.8" customHeight="1" s="12">
@@ -12445,7 +12445,7 @@
       </c>
       <c r="C15" s="14" t="inlineStr">
         <is>
-          <t>MultiRefOffCentre</t>
+          <t>LOSMovedBox</t>
         </is>
       </c>
     </row>
@@ -22110,19 +22110,22 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="8.67" customWidth="1" style="11" min="1" max="1025"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15" customHeight="1" s="12">
       <c r="A1" s="11" t="n">
         <v>0</v>
       </c>
@@ -22133,7 +22136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15" customHeight="1" s="12">
       <c r="A2" s="11" t="n">
         <v>0.766044443118978</v>
       </c>
@@ -22144,7 +22147,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15" customHeight="1" s="12">
       <c r="A3" s="11" t="n">
         <v>0.3830222215594891</v>
       </c>
@@ -22155,7 +22158,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15" customHeight="1" s="12">
       <c r="A4" s="11" t="n">
         <v>-0.3830222215594888</v>
       </c>
@@ -22166,7 +22169,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15" customHeight="1" s="12">
       <c r="A5" s="11" t="n">
         <v>-0.766044443118978</v>
       </c>
@@ -22177,7 +22180,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15" customHeight="1" s="12">
       <c r="A6" s="11" t="n">
         <v>-0.3830222215594893</v>
       </c>
@@ -22188,7 +22191,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="15" customHeight="1" s="12">
       <c r="A7" s="11" t="n">
         <v>0.3830222215594885</v>
       </c>
@@ -22199,7 +22202,7 @@
         <v>0.6427876096865393</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="15" customHeight="1" s="12">
       <c r="A8" s="11" t="n">
         <v>1</v>
       </c>
@@ -22210,7 +22213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="15" customHeight="1" s="12">
       <c r="A9" s="11" t="n">
         <v>0.7071067811865476</v>
       </c>
@@ -22221,7 +22224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="15" customHeight="1" s="12">
       <c r="A10" s="11" t="n">
         <v>6.123233995736766e-17</v>
       </c>
@@ -22232,7 +22235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="15" customHeight="1" s="12">
       <c r="A11" s="11" t="n">
         <v>-0.7071067811865475</v>
       </c>
@@ -22243,7 +22246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="15" customHeight="1" s="12">
       <c r="A12" s="11" t="n">
         <v>-1</v>
       </c>
@@ -22254,7 +22257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="15" customHeight="1" s="12">
       <c r="A13" s="11" t="n">
         <v>-0.7071067811865477</v>
       </c>
@@ -22265,7 +22268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="15" customHeight="1" s="12">
       <c r="A14" s="11" t="n">
         <v>-1.83697019872103e-16</v>
       </c>
@@ -22276,7 +22279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" ht="15" customHeight="1" s="12">
       <c r="A15" s="11" t="n">
         <v>0.7071067811865474</v>
       </c>
@@ -22287,7 +22290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="15" customHeight="1" s="12">
       <c r="A16" s="11" t="n">
         <v>0.766044443118978</v>
       </c>
@@ -22298,7 +22301,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" ht="15" customHeight="1" s="12">
       <c r="A17" s="11" t="n">
         <v>0.3830222215594891</v>
       </c>
@@ -22309,7 +22312,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" ht="15" customHeight="1" s="12">
       <c r="A18" s="11" t="n">
         <v>-0.3830222215594888</v>
       </c>
@@ -22320,7 +22323,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="15" customHeight="1" s="12">
       <c r="A19" s="11" t="n">
         <v>-0.766044443118978</v>
       </c>
@@ -22331,7 +22334,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" ht="15" customHeight="1" s="12">
       <c r="A20" s="11" t="n">
         <v>-0.3830222215594893</v>
       </c>
@@ -22342,7 +22345,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" ht="15" customHeight="1" s="12">
       <c r="A21" s="11" t="n">
         <v>0.3830222215594885</v>
       </c>
@@ -22353,7 +22356,7 @@
         <v>-0.6427876096865393</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" ht="15" customHeight="1" s="12">
       <c r="A22" s="11" t="n">
         <v>0</v>
       </c>
@@ -22365,7 +22368,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
@@ -22569,7 +22574,7 @@
       </c>
       <c r="E3" s="11" t="inlineStr">
         <is>
-          <t>(0.8855548599197771+0.005952846860713298j)</t>
+          <t>(0.8855885559191065+0.003942667577037837j)</t>
         </is>
       </c>
     </row>
@@ -22590,8 +22595,8 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -22709,16 +22714,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="F2" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G2" s="11" t="n">
         <v>0.45</v>
       </c>
-      <c r="G2" s="11" t="n">
-        <v>0</v>
-      </c>
       <c r="H2" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="I2" s="11" t="n">
         <v>0</v>
@@ -23436,10 +23441,10 @@
         </is>
       </c>
       <c r="B34" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C34" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D34" s="11" t="n">
         <v>0</v>
@@ -23447,10 +23452,10 @@
     </row>
     <row r="35" ht="15" customHeight="1" s="12">
       <c r="B35" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C35" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D35" s="11" t="n">
         <v>0</v>
@@ -23458,10 +23463,10 @@
     </row>
     <row r="36" ht="15" customHeight="1" s="12">
       <c r="B36" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C36" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D36" s="11" t="n">
         <v>0.45</v>
@@ -23470,14 +23475,14 @@
     <row r="37" ht="15" customHeight="1" s="12">
       <c r="A37" s="11" t="inlineStr">
         <is>
-          <t>Obstacle12</t>
+          <t>Obstacle012</t>
         </is>
       </c>
       <c r="B37" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C37" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D37" s="11" t="n">
         <v>0</v>
@@ -23485,10 +23490,10 @@
     </row>
     <row r="38" ht="15" customHeight="1" s="12">
       <c r="B38" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C38" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C38" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D38" s="11" t="n">
         <v>0</v>
@@ -23496,10 +23501,10 @@
     </row>
     <row r="39" ht="15" customHeight="1" s="12">
       <c r="B39" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C39" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D39" s="11" t="n">
         <v>0.45</v>
@@ -23508,14 +23513,14 @@
     <row r="40" ht="15" customHeight="1" s="12">
       <c r="A40" s="11" t="inlineStr">
         <is>
-          <t>Obstacle13</t>
+          <t>Obstacle013</t>
         </is>
       </c>
       <c r="B40" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C40" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D40" s="11" t="n">
         <v>0.45</v>
@@ -23523,10 +23528,10 @@
     </row>
     <row r="41" ht="15" customHeight="1" s="12">
       <c r="B41" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C41" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C41" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D41" s="11" t="n">
         <v>0.45</v>
@@ -23534,10 +23539,10 @@
     </row>
     <row r="42" ht="15" customHeight="1" s="12">
       <c r="B42" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C42" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C42" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D42" s="11" t="n">
         <v>0</v>
@@ -23546,14 +23551,14 @@
     <row r="43" ht="15" customHeight="1" s="12">
       <c r="A43" s="11" t="inlineStr">
         <is>
-          <t>Obstacle14</t>
+          <t>Obstacle014</t>
         </is>
       </c>
       <c r="B43" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C43" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D43" s="11" t="n">
         <v>0</v>
@@ -23561,10 +23566,10 @@
     </row>
     <row r="44" ht="15" customHeight="1" s="12">
       <c r="B44" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C44" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D44" s="11" t="n">
         <v>0</v>
@@ -23572,10 +23577,10 @@
     </row>
     <row r="45" ht="15" customHeight="1" s="12">
       <c r="B45" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C45" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D45" s="11" t="n">
         <v>0.45</v>
@@ -23584,14 +23589,14 @@
     <row r="46" ht="15" customHeight="1" s="12">
       <c r="A46" s="11" t="inlineStr">
         <is>
-          <t>Obstacle15</t>
+          <t>Obstacle015</t>
         </is>
       </c>
       <c r="B46" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C46" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D46" s="11" t="n">
         <v>0.45</v>
@@ -23599,10 +23604,10 @@
     </row>
     <row r="47" ht="15" customHeight="1" s="12">
       <c r="B47" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C47" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D47" s="11" t="n">
         <v>0</v>
@@ -23610,10 +23615,10 @@
     </row>
     <row r="48" ht="15" customHeight="1" s="12">
       <c r="B48" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C48" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D48" s="11" t="n">
         <v>0.45</v>
@@ -23622,14 +23627,14 @@
     <row r="49" ht="15" customHeight="1" s="12">
       <c r="A49" s="11" t="inlineStr">
         <is>
-          <t>Obstacle16</t>
+          <t>Obstacle016</t>
         </is>
       </c>
       <c r="B49" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C49" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D49" s="11" t="n">
         <v>0</v>
@@ -23637,10 +23642,10 @@
     </row>
     <row r="50" ht="15" customHeight="1" s="12">
       <c r="B50" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C50" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D50" s="11" t="n">
         <v>0</v>
@@ -23648,10 +23653,10 @@
     </row>
     <row r="51" ht="15" customHeight="1" s="12">
       <c r="B51" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C51" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D51" s="11" t="n">
         <v>0</v>
@@ -23660,14 +23665,14 @@
     <row r="52" ht="15" customHeight="1" s="12">
       <c r="A52" s="11" t="inlineStr">
         <is>
-          <t>Obstacle17</t>
+          <t>Obstacle017</t>
         </is>
       </c>
       <c r="B52" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C52" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D52" s="11" t="n">
         <v>0</v>
@@ -23675,10 +23680,10 @@
     </row>
     <row r="53" ht="15" customHeight="1" s="12">
       <c r="B53" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C53" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D53" s="11" t="n">
         <v>0</v>
@@ -23686,10 +23691,10 @@
     </row>
     <row r="54" ht="15" customHeight="1" s="12">
       <c r="B54" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C54" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C54" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D54" s="11" t="n">
         <v>0</v>
@@ -23698,14 +23703,14 @@
     <row r="55" ht="15" customHeight="1" s="12">
       <c r="A55" s="11" t="inlineStr">
         <is>
-          <t>Obstacle18</t>
+          <t>Obstacle018</t>
         </is>
       </c>
       <c r="B55" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C55" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D55" s="11" t="n">
         <v>0.45</v>
@@ -23713,10 +23718,10 @@
     </row>
     <row r="56" ht="15" customHeight="1" s="12">
       <c r="B56" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C56" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D56" s="11" t="n">
         <v>0.45</v>
@@ -23724,10 +23729,10 @@
     </row>
     <row r="57" ht="15" customHeight="1" s="12">
       <c r="B57" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C57" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C57" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D57" s="11" t="n">
         <v>0.45</v>
@@ -23736,14 +23741,14 @@
     <row r="58" ht="15" customHeight="1" s="12">
       <c r="A58" s="11" t="inlineStr">
         <is>
-          <t>Obstacle19</t>
+          <t>Obstacle019</t>
         </is>
       </c>
       <c r="B58" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C58" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D58" s="11" t="n">
         <v>0.45</v>
@@ -23751,10 +23756,10 @@
     </row>
     <row r="59" ht="15" customHeight="1" s="12">
       <c r="B59" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C59" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D59" s="11" t="n">
         <v>0.45</v>
@@ -23762,10 +23767,10 @@
     </row>
     <row r="60" ht="15" customHeight="1" s="12">
       <c r="B60" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C60" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D60" s="11" t="n">
         <v>0.45</v>
@@ -23774,14 +23779,14 @@
     <row r="61" ht="15" customHeight="1" s="12">
       <c r="A61" s="11" t="inlineStr">
         <is>
-          <t>Obstacle20</t>
+          <t>Obstacle020</t>
         </is>
       </c>
       <c r="B61" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C61" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C61" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D61" s="11" t="n">
         <v>0.45</v>
@@ -23789,10 +23794,10 @@
     </row>
     <row r="62" ht="15" customHeight="1" s="12">
       <c r="B62" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C62" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D62" s="11" t="n">
         <v>0.45</v>
@@ -23800,10 +23805,10 @@
     </row>
     <row r="63" ht="15" customHeight="1" s="12">
       <c r="B63" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C63" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D63" s="11" t="n">
         <v>0</v>
@@ -23812,14 +23817,14 @@
     <row r="64" ht="15" customHeight="1" s="12">
       <c r="A64" s="11" t="inlineStr">
         <is>
-          <t>Obstacle21</t>
+          <t>Obstacle021</t>
         </is>
       </c>
       <c r="B64" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C64" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C64" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D64" s="11" t="n">
         <v>0.45</v>
@@ -23827,10 +23832,10 @@
     </row>
     <row r="65" ht="15" customHeight="1" s="12">
       <c r="B65" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C65" s="11" t="n">
         <v>0.45</v>
-      </c>
-      <c r="C65" s="11" t="n">
-        <v>0</v>
       </c>
       <c r="D65" s="11" t="n">
         <v>0</v>
@@ -23838,10 +23843,10 @@
     </row>
     <row r="66" ht="15" customHeight="1" s="12">
       <c r="B66" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C66" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D66" s="11" t="n">
         <v>0</v>
@@ -23850,14 +23855,14 @@
     <row r="67" ht="15" customHeight="1" s="12">
       <c r="A67" s="11" t="inlineStr">
         <is>
-          <t>Obstacle22</t>
+          <t>Obstacle022</t>
         </is>
       </c>
       <c r="B67" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C67" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D67" s="11" t="n">
         <v>0</v>
@@ -23865,10 +23870,10 @@
     </row>
     <row r="68" ht="15" customHeight="1" s="12">
       <c r="B68" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C68" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D68" s="11" t="n">
         <v>0.45</v>
@@ -23876,10 +23881,10 @@
     </row>
     <row r="69" ht="15" customHeight="1" s="12">
       <c r="B69" s="11" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C69" s="11" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="D69" s="11" t="n">
         <v>0.45</v>

</xml_diff>

<commit_message>
Changed ray number to start at 98 to see if this reveals shadow areas.
</commit_message>
<xml_diff>
--- a/ParameterIndependent/InputSheet.xlsx
+++ b/ParameterIndependent/InputSheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AngleSpacing" sheetId="1" state="visible" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Directions282" sheetId="21" state="visible" r:id="rId21"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Directions337" sheetId="22" state="visible" r:id="rId22"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Directions022" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Directions098" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -515,8 +516,8 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="10:14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -538,108 +539,113 @@
     </row>
     <row r="2" ht="14.4" customHeight="1" s="12">
       <c r="A2" s="11" t="n">
-        <v>0.7853981633974479</v>
+        <v>0.349065850398866</v>
       </c>
       <c r="B2" s="11" t="n">
-        <v>22</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" ht="14.4" customHeight="1" s="12">
       <c r="A3" s="11" t="n">
-        <v>0.628318530717959</v>
+        <v>0.314159265358979</v>
       </c>
       <c r="B3" s="11" t="n">
-        <v>32</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" ht="14.4" customHeight="1" s="12">
       <c r="A4" s="11" t="n">
-        <v>0.523598775598299</v>
+        <v>0.285599332144527</v>
       </c>
       <c r="B4" s="11" t="n">
-        <v>44</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" ht="14.4" customHeight="1" s="12">
       <c r="A5" s="11" t="n">
-        <v>0.448798950512828</v>
+        <v>0.261799387799149</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>56</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" ht="14.4" customHeight="1" s="12">
       <c r="A6" s="11" t="n">
-        <v>0.392699081698724</v>
+        <v>0.241660973353061</v>
       </c>
       <c r="B6" s="11" t="n">
-        <v>87</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" ht="14.4" customHeight="1" s="12">
       <c r="A7" s="11" t="n">
-        <v>0.349065850398866</v>
+        <v>0.224399475256414</v>
       </c>
       <c r="B7" s="11" t="n">
-        <v>98</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" ht="14.4" customHeight="1" s="12">
       <c r="A8" s="11" t="n">
-        <v>0.314159265358979</v>
+        <v>0.20943951023932</v>
       </c>
       <c r="B8" s="11" t="n">
-        <v>136</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" ht="14.4" customHeight="1" s="12">
       <c r="A9" s="11" t="n">
-        <v>0.285599332144527</v>
+        <v>0.196349540849362</v>
       </c>
       <c r="B9" s="11" t="n">
-        <v>149</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" ht="14.4" customHeight="1" s="12">
       <c r="A10" s="11" t="n">
-        <v>0.261799387799149</v>
+        <v>0.7853981633974479</v>
       </c>
       <c r="B10" s="11" t="n">
-        <v>192</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" ht="14.4" customHeight="1" s="12">
       <c r="A11" s="11" t="n">
-        <v>0.241660973353061</v>
+        <v>0.628318530717959</v>
       </c>
       <c r="B11" s="11" t="n">
-        <v>211</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" ht="14.4" customHeight="1" s="12">
       <c r="A12" s="11" t="n">
-        <v>0.224399475256414</v>
+        <v>0.523598775598299</v>
       </c>
       <c r="B12" s="11" t="n">
-        <v>244</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" ht="14.4" customHeight="1" s="12">
       <c r="A13" s="11" t="n">
-        <v>0.20943951023932</v>
+        <v>0.448798950512828</v>
       </c>
       <c r="B13" s="11" t="n">
-        <v>282</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" ht="14.4" customHeight="1" s="12">
       <c r="A14" s="11" t="n">
-        <v>0.196349540849362</v>
+        <v>0.392699081698724</v>
       </c>
       <c r="B14" s="11" t="n">
-        <v>337</v>
-      </c>
-    </row>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="1048570" ht="12.8" customHeight="1" s="12"/>
+    <row r="1048571" ht="12.8" customHeight="1" s="12"/>
+    <row r="1048572" ht="12.8" customHeight="1" s="12"/>
+    <row r="1048573" ht="12.8" customHeight="1" s="12"/>
+    <row r="1048574" ht="12.8" customHeight="1" s="12"/>
     <row r="1048575" ht="12.8" customHeight="1" s="12"/>
     <row r="1048576" ht="12.8" customHeight="1" s="12"/>
   </sheetData>
@@ -658,7 +664,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -924,7 +930,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -1300,7 +1306,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -1808,7 +1814,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -2448,7 +2454,7 @@
   <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -3429,7 +3435,7 @@
   <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -4531,7 +4537,7 @@
   <dimension ref="A1:C136"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -6051,7 +6057,7 @@
   <dimension ref="A1:C149"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -7714,7 +7720,7 @@
   <dimension ref="A1:C192"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -9850,7 +9856,7 @@
   <dimension ref="A1:C211"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -12194,8 +12200,8 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="10:14 C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -12552,7 +12558,7 @@
   <dimension ref="A1:C244"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -15260,7 +15266,7 @@
   <dimension ref="A1:C282"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -18386,7 +18392,7 @@
   <dimension ref="A1:C337"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -22117,7 +22123,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -22144,29 +22150,29 @@
         <v>0</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="12">
       <c r="A3" s="11" t="n">
-        <v>0.3830222215594891</v>
+        <v>0.383022221559489</v>
       </c>
       <c r="B3" s="11" t="n">
-        <v>0.6634139481689384</v>
+        <v>0.663413948168938</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="12">
       <c r="A4" s="11" t="n">
-        <v>-0.3830222215594888</v>
+        <v>-0.383022221559489</v>
       </c>
       <c r="B4" s="11" t="n">
-        <v>0.6634139481689384</v>
+        <v>0.663413948168938</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="12">
@@ -22174,32 +22180,32 @@
         <v>-0.766044443118978</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>9.381338752702731e-17</v>
+        <v>9.38133875270273e-17</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="12">
       <c r="A6" s="11" t="n">
-        <v>-0.3830222215594893</v>
+        <v>-0.383022221559489</v>
       </c>
       <c r="B6" s="11" t="n">
-        <v>-0.6634139481689382</v>
+        <v>-0.663413948168938</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="12">
       <c r="A7" s="11" t="n">
-        <v>0.3830222215594885</v>
+        <v>0.383022221559489</v>
       </c>
       <c r="B7" s="11" t="n">
-        <v>-0.6634139481689387</v>
+        <v>-0.6634139481689389</v>
       </c>
       <c r="C7" s="11" t="n">
-        <v>0.6427876096865393</v>
+        <v>0.642787609686539</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="12">
@@ -22215,10 +22221,10 @@
     </row>
     <row r="9" ht="15" customHeight="1" s="12">
       <c r="A9" s="11" t="n">
-        <v>0.7071067811865476</v>
+        <v>0.707106781186548</v>
       </c>
       <c r="B9" s="11" t="n">
-        <v>0.7071067811865475</v>
+        <v>0.707106781186547</v>
       </c>
       <c r="C9" s="11" t="n">
         <v>0</v>
@@ -22226,7 +22232,7 @@
     </row>
     <row r="10" ht="15" customHeight="1" s="12">
       <c r="A10" s="11" t="n">
-        <v>6.123233995736766e-17</v>
+        <v>6.12323399573677e-17</v>
       </c>
       <c r="B10" s="11" t="n">
         <v>1</v>
@@ -22237,10 +22243,10 @@
     </row>
     <row r="11" ht="15" customHeight="1" s="12">
       <c r="A11" s="11" t="n">
-        <v>-0.7071067811865475</v>
+        <v>-0.707106781186547</v>
       </c>
       <c r="B11" s="11" t="n">
-        <v>0.7071067811865476</v>
+        <v>0.707106781186548</v>
       </c>
       <c r="C11" s="11" t="n">
         <v>0</v>
@@ -22251,7 +22257,7 @@
         <v>-1</v>
       </c>
       <c r="B12" s="11" t="n">
-        <v>1.224646799147353e-16</v>
+        <v>1.22464679914735e-16</v>
       </c>
       <c r="C12" s="11" t="n">
         <v>0</v>
@@ -22259,10 +22265,10 @@
     </row>
     <row r="13" ht="15" customHeight="1" s="12">
       <c r="A13" s="11" t="n">
-        <v>-0.7071067811865477</v>
+        <v>-0.707106781186548</v>
       </c>
       <c r="B13" s="11" t="n">
-        <v>-0.7071067811865475</v>
+        <v>-0.707106781186547</v>
       </c>
       <c r="C13" s="11" t="n">
         <v>0</v>
@@ -22281,10 +22287,10 @@
     </row>
     <row r="15" ht="15" customHeight="1" s="12">
       <c r="A15" s="11" t="n">
-        <v>0.7071067811865474</v>
+        <v>0.707106781186547</v>
       </c>
       <c r="B15" s="11" t="n">
-        <v>-0.7071067811865477</v>
+        <v>-0.707106781186548</v>
       </c>
       <c r="C15" s="11" t="n">
         <v>0</v>
@@ -22298,29 +22304,29 @@
         <v>0</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="12">
       <c r="A17" s="11" t="n">
-        <v>0.3830222215594891</v>
+        <v>0.383022221559489</v>
       </c>
       <c r="B17" s="11" t="n">
-        <v>0.6634139481689384</v>
+        <v>0.663413948168938</v>
       </c>
       <c r="C17" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="12">
       <c r="A18" s="11" t="n">
-        <v>-0.3830222215594888</v>
+        <v>-0.383022221559489</v>
       </c>
       <c r="B18" s="11" t="n">
-        <v>0.6634139481689384</v>
+        <v>0.663413948168938</v>
       </c>
       <c r="C18" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="12">
@@ -22328,32 +22334,32 @@
         <v>-0.766044443118978</v>
       </c>
       <c r="B19" s="11" t="n">
-        <v>9.381338752702731e-17</v>
+        <v>9.38133875270273e-17</v>
       </c>
       <c r="C19" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="12">
       <c r="A20" s="11" t="n">
-        <v>-0.3830222215594893</v>
+        <v>-0.383022221559489</v>
       </c>
       <c r="B20" s="11" t="n">
-        <v>-0.6634139481689382</v>
+        <v>-0.663413948168938</v>
       </c>
       <c r="C20" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="12">
       <c r="A21" s="11" t="n">
-        <v>0.3830222215594885</v>
+        <v>0.383022221559489</v>
       </c>
       <c r="B21" s="11" t="n">
-        <v>-0.6634139481689387</v>
+        <v>-0.6634139481689389</v>
       </c>
       <c r="C21" s="11" t="n">
-        <v>-0.6427876096865393</v>
+        <v>-0.642787609686539</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="12">
@@ -22371,6 +22377,1103 @@
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="n">
+        <v>0.1736481776669304</v>
+      </c>
+      <c r="B2" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11" t="n">
+        <v>0.984807753012208</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="n">
+        <v>-0.1736481776669304</v>
+      </c>
+      <c r="B3" s="11" t="n">
+        <v>2.126576849575772e-17</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>0.984807753012208</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="n">
+        <v>0.5000000000000001</v>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11" t="n">
+        <v>0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="n">
+        <v>0.3535533905932738</v>
+      </c>
+      <c r="B5" s="11" t="n">
+        <v>0.3535533905932738</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <v>0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="n">
+        <v>3.061616997868384e-17</v>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>0.5000000000000001</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="11" t="n">
+        <v>-0.3535533905932738</v>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>0.3535533905932738</v>
+      </c>
+      <c r="C7" s="11" t="n">
+        <v>0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="n">
+        <v>-0.5000000000000001</v>
+      </c>
+      <c r="B8" s="11" t="n">
+        <v>6.123233995736767e-17</v>
+      </c>
+      <c r="C8" s="11" t="n">
+        <v>0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="n">
+        <v>-0.3535533905932739</v>
+      </c>
+      <c r="B9" s="11" t="n">
+        <v>-0.3535533905932738</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="n">
+        <v>-9.184850993605151e-17</v>
+      </c>
+      <c r="B10" s="11" t="n">
+        <v>-0.5000000000000001</v>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="n">
+        <v>0.3535533905932737</v>
+      </c>
+      <c r="B11" s="11" t="n">
+        <v>-0.3535533905932739</v>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="n">
+        <v>0.766044443118978</v>
+      </c>
+      <c r="B12" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="11" t="n">
+        <v>0.6782986680778567</v>
+      </c>
+      <c r="B13" s="11" t="n">
+        <v>0.3559986035327536</v>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="11" t="n">
+        <v>0.4351628425651916</v>
+      </c>
+      <c r="B14" s="11" t="n">
+        <v>0.6304422172444096</v>
+      </c>
+      <c r="C14" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="11" t="n">
+        <v>0.09233645410159939</v>
+      </c>
+      <c r="B15" s="11" t="n">
+        <v>0.7604591166377114</v>
+      </c>
+      <c r="C15" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="11" t="n">
+        <v>-0.2716431032217672</v>
+      </c>
+      <c r="B16" s="11" t="n">
+        <v>0.7162639969351478</v>
+      </c>
+      <c r="C16" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="11" t="n">
+        <v>-0.5733924992513005</v>
+      </c>
+      <c r="B17" s="11" t="n">
+        <v>0.5079814274516465</v>
+      </c>
+      <c r="C17" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="n">
+        <v>-0.7437845838310684</v>
+      </c>
+      <c r="B18" s="11" t="n">
+        <v>0.1833264347788107</v>
+      </c>
+      <c r="C18" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="n">
+        <v>-0.7437845838310685</v>
+      </c>
+      <c r="B19" s="11" t="n">
+        <v>-0.1833264347788102</v>
+      </c>
+      <c r="C19" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="n">
+        <v>-0.5733924992513009</v>
+      </c>
+      <c r="B20" s="11" t="n">
+        <v>-0.5079814274516462</v>
+      </c>
+      <c r="C20" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="11" t="n">
+        <v>-0.2716431032217675</v>
+      </c>
+      <c r="B21" s="11" t="n">
+        <v>-0.7162639969351478</v>
+      </c>
+      <c r="C21" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="11" t="n">
+        <v>0.0923364541015987</v>
+      </c>
+      <c r="B22" s="11" t="n">
+        <v>-0.7604591166377115</v>
+      </c>
+      <c r="C22" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="11" t="n">
+        <v>0.4351628425651914</v>
+      </c>
+      <c r="B23" s="11" t="n">
+        <v>-0.6304422172444099</v>
+      </c>
+      <c r="C23" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="11" t="n">
+        <v>0.6782986680778564</v>
+      </c>
+      <c r="B24" s="11" t="n">
+        <v>-0.3559986035327541</v>
+      </c>
+      <c r="C24" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="11" t="n">
+        <v>0.9396926207859084</v>
+      </c>
+      <c r="B25" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="11" t="n">
+        <v>0.8681627791959909</v>
+      </c>
+      <c r="B26" s="11" t="n">
+        <v>0.3596047974904982</v>
+      </c>
+      <c r="C26" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="11" t="n">
+        <v>0.6644630243886748</v>
+      </c>
+      <c r="B27" s="11" t="n">
+        <v>0.6644630243886747</v>
+      </c>
+      <c r="C27" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="11" t="n">
+        <v>0.3596047974904982</v>
+      </c>
+      <c r="B28" s="11" t="n">
+        <v>0.8681627791959909</v>
+      </c>
+      <c r="C28" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="11" t="n">
+        <v>5.753957801139251e-17</v>
+      </c>
+      <c r="B29" s="11" t="n">
+        <v>0.9396926207859084</v>
+      </c>
+      <c r="C29" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="11" t="n">
+        <v>-0.3596047974904981</v>
+      </c>
+      <c r="B30" s="11" t="n">
+        <v>0.8681627791959909</v>
+      </c>
+      <c r="C30" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="11" t="n">
+        <v>-0.6644630243886747</v>
+      </c>
+      <c r="B31" s="11" t="n">
+        <v>0.6644630243886748</v>
+      </c>
+      <c r="C31" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="11" t="n">
+        <v>-0.8681627791959909</v>
+      </c>
+      <c r="B32" s="11" t="n">
+        <v>0.3596047974904982</v>
+      </c>
+      <c r="C32" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="11" t="n">
+        <v>-0.9396926207859084</v>
+      </c>
+      <c r="B33" s="11" t="n">
+        <v>1.15079156022785e-16</v>
+      </c>
+      <c r="C33" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="11" t="n">
+        <v>-0.8681627791959911</v>
+      </c>
+      <c r="B34" s="11" t="n">
+        <v>-0.3596047974904981</v>
+      </c>
+      <c r="C34" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="11" t="n">
+        <v>-0.6644630243886749</v>
+      </c>
+      <c r="B35" s="11" t="n">
+        <v>-0.6644630243886747</v>
+      </c>
+      <c r="C35" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="11" t="n">
+        <v>-0.3596047974904987</v>
+      </c>
+      <c r="B36" s="11" t="n">
+        <v>-0.8681627791959907</v>
+      </c>
+      <c r="C36" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="11" t="n">
+        <v>-1.726187340341775e-16</v>
+      </c>
+      <c r="B37" s="11" t="n">
+        <v>-0.9396926207859084</v>
+      </c>
+      <c r="C37" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="11" t="n">
+        <v>0.3596047974904983</v>
+      </c>
+      <c r="B38" s="11" t="n">
+        <v>-0.8681627791959908</v>
+      </c>
+      <c r="C38" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="11" t="n">
+        <v>0.6644630243886746</v>
+      </c>
+      <c r="B39" s="11" t="n">
+        <v>-0.6644630243886749</v>
+      </c>
+      <c r="C39" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="11" t="n">
+        <v>0.8681627791959907</v>
+      </c>
+      <c r="B40" s="11" t="n">
+        <v>-0.3596047974904987</v>
+      </c>
+      <c r="C40" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B41" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="11" t="n">
+        <v>0.9396926207859084</v>
+      </c>
+      <c r="B42" s="11" t="n">
+        <v>0.3420201433256687</v>
+      </c>
+      <c r="C42" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="11" t="n">
+        <v>0.766044443118978</v>
+      </c>
+      <c r="B43" s="11" t="n">
+        <v>0.6427876096865393</v>
+      </c>
+      <c r="C43" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="11" t="n">
+        <v>0.5000000000000001</v>
+      </c>
+      <c r="B44" s="11" t="n">
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="C44" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="11" t="n">
+        <v>0.1736481776669304</v>
+      </c>
+      <c r="B45" s="11" t="n">
+        <v>0.984807753012208</v>
+      </c>
+      <c r="C45" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="11" t="n">
+        <v>-0.1736481776669303</v>
+      </c>
+      <c r="B46" s="11" t="n">
+        <v>0.984807753012208</v>
+      </c>
+      <c r="C46" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="11" t="n">
+        <v>-0.4999999999999998</v>
+      </c>
+      <c r="B47" s="11" t="n">
+        <v>0.8660254037844387</v>
+      </c>
+      <c r="C47" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="11" t="n">
+        <v>-0.7660444431189779</v>
+      </c>
+      <c r="B48" s="11" t="n">
+        <v>0.6427876096865395</v>
+      </c>
+      <c r="C48" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="11" t="n">
+        <v>-0.9396926207859083</v>
+      </c>
+      <c r="B49" s="11" t="n">
+        <v>0.3420201433256689</v>
+      </c>
+      <c r="C49" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="B50" s="11" t="n">
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="C50" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="11" t="n">
+        <v>-0.9396926207859084</v>
+      </c>
+      <c r="B51" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+      <c r="C51" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="11" t="n">
+        <v>-0.766044443118978</v>
+      </c>
+      <c r="B52" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+      <c r="C52" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="11" t="n">
+        <v>-0.5000000000000004</v>
+      </c>
+      <c r="B53" s="11" t="n">
+        <v>-0.8660254037844384</v>
+      </c>
+      <c r="C53" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="11" t="n">
+        <v>-0.1736481776669303</v>
+      </c>
+      <c r="B54" s="11" t="n">
+        <v>-0.984807753012208</v>
+      </c>
+      <c r="C54" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="11" t="n">
+        <v>0.17364817766693</v>
+      </c>
+      <c r="B55" s="11" t="n">
+        <v>-0.9848077530122081</v>
+      </c>
+      <c r="C55" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="11" t="n">
+        <v>0.5000000000000001</v>
+      </c>
+      <c r="B56" s="11" t="n">
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="C56" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="11" t="n">
+        <v>0.7660444431189778</v>
+      </c>
+      <c r="B57" s="11" t="n">
+        <v>-0.6427876096865396</v>
+      </c>
+      <c r="C57" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="11" t="n">
+        <v>0.9396926207859081</v>
+      </c>
+      <c r="B58" s="11" t="n">
+        <v>-0.3420201433256694</v>
+      </c>
+      <c r="C58" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="11" t="n">
+        <v>0.9396926207859084</v>
+      </c>
+      <c r="B59" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="11" t="n">
+        <v>0.8681627791959909</v>
+      </c>
+      <c r="B60" s="11" t="n">
+        <v>0.3596047974904982</v>
+      </c>
+      <c r="C60" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="11" t="n">
+        <v>0.6644630243886748</v>
+      </c>
+      <c r="B61" s="11" t="n">
+        <v>0.6644630243886747</v>
+      </c>
+      <c r="C61" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="11" t="n">
+        <v>0.3596047974904982</v>
+      </c>
+      <c r="B62" s="11" t="n">
+        <v>0.8681627791959909</v>
+      </c>
+      <c r="C62" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="11" t="n">
+        <v>5.753957801139251e-17</v>
+      </c>
+      <c r="B63" s="11" t="n">
+        <v>0.9396926207859084</v>
+      </c>
+      <c r="C63" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="11" t="n">
+        <v>-0.3596047974904981</v>
+      </c>
+      <c r="B64" s="11" t="n">
+        <v>0.8681627791959909</v>
+      </c>
+      <c r="C64" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="11" t="n">
+        <v>-0.6644630243886747</v>
+      </c>
+      <c r="B65" s="11" t="n">
+        <v>0.6644630243886748</v>
+      </c>
+      <c r="C65" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="11" t="n">
+        <v>-0.8681627791959909</v>
+      </c>
+      <c r="B66" s="11" t="n">
+        <v>0.3596047974904982</v>
+      </c>
+      <c r="C66" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="11" t="n">
+        <v>-0.9396926207859084</v>
+      </c>
+      <c r="B67" s="11" t="n">
+        <v>1.15079156022785e-16</v>
+      </c>
+      <c r="C67" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="11" t="n">
+        <v>-0.8681627791959911</v>
+      </c>
+      <c r="B68" s="11" t="n">
+        <v>-0.3596047974904981</v>
+      </c>
+      <c r="C68" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="11" t="n">
+        <v>-0.6644630243886749</v>
+      </c>
+      <c r="B69" s="11" t="n">
+        <v>-0.6644630243886747</v>
+      </c>
+      <c r="C69" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="11" t="n">
+        <v>-0.3596047974904987</v>
+      </c>
+      <c r="B70" s="11" t="n">
+        <v>-0.8681627791959907</v>
+      </c>
+      <c r="C70" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="11" t="n">
+        <v>-1.726187340341775e-16</v>
+      </c>
+      <c r="B71" s="11" t="n">
+        <v>-0.9396926207859084</v>
+      </c>
+      <c r="C71" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="11" t="n">
+        <v>0.3596047974904983</v>
+      </c>
+      <c r="B72" s="11" t="n">
+        <v>-0.8681627791959908</v>
+      </c>
+      <c r="C72" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="11" t="n">
+        <v>0.6644630243886746</v>
+      </c>
+      <c r="B73" s="11" t="n">
+        <v>-0.6644630243886749</v>
+      </c>
+      <c r="C73" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="11" t="n">
+        <v>0.8681627791959907</v>
+      </c>
+      <c r="B74" s="11" t="n">
+        <v>-0.3596047974904987</v>
+      </c>
+      <c r="C74" s="11" t="n">
+        <v>-0.3420201433256687</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="11" t="n">
+        <v>0.766044443118978</v>
+      </c>
+      <c r="B75" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C75" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="11" t="n">
+        <v>0.6782986680778567</v>
+      </c>
+      <c r="B76" s="11" t="n">
+        <v>0.3559986035327536</v>
+      </c>
+      <c r="C76" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="11" t="n">
+        <v>0.4351628425651916</v>
+      </c>
+      <c r="B77" s="11" t="n">
+        <v>0.6304422172444096</v>
+      </c>
+      <c r="C77" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="11" t="n">
+        <v>0.09233645410159939</v>
+      </c>
+      <c r="B78" s="11" t="n">
+        <v>0.7604591166377114</v>
+      </c>
+      <c r="C78" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="11" t="n">
+        <v>-0.2716431032217672</v>
+      </c>
+      <c r="B79" s="11" t="n">
+        <v>0.7162639969351478</v>
+      </c>
+      <c r="C79" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="11" t="n">
+        <v>-0.5733924992513005</v>
+      </c>
+      <c r="B80" s="11" t="n">
+        <v>0.5079814274516465</v>
+      </c>
+      <c r="C80" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="11" t="n">
+        <v>-0.7437845838310684</v>
+      </c>
+      <c r="B81" s="11" t="n">
+        <v>0.1833264347788107</v>
+      </c>
+      <c r="C81" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="11" t="n">
+        <v>-0.7437845838310685</v>
+      </c>
+      <c r="B82" s="11" t="n">
+        <v>-0.1833264347788102</v>
+      </c>
+      <c r="C82" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="11" t="n">
+        <v>-0.5733924992513009</v>
+      </c>
+      <c r="B83" s="11" t="n">
+        <v>-0.5079814274516462</v>
+      </c>
+      <c r="C83" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="11" t="n">
+        <v>-0.2716431032217675</v>
+      </c>
+      <c r="B84" s="11" t="n">
+        <v>-0.7162639969351478</v>
+      </c>
+      <c r="C84" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="11" t="n">
+        <v>0.0923364541015987</v>
+      </c>
+      <c r="B85" s="11" t="n">
+        <v>-0.7604591166377115</v>
+      </c>
+      <c r="C85" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="11" t="n">
+        <v>0.4351628425651914</v>
+      </c>
+      <c r="B86" s="11" t="n">
+        <v>-0.6304422172444099</v>
+      </c>
+      <c r="C86" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="11" t="n">
+        <v>0.6782986680778564</v>
+      </c>
+      <c r="B87" s="11" t="n">
+        <v>-0.3559986035327541</v>
+      </c>
+      <c r="C87" s="11" t="n">
+        <v>-0.6427876096865393</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="11" t="n">
+        <v>0.5000000000000001</v>
+      </c>
+      <c r="B88" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C88" s="11" t="n">
+        <v>-0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="11" t="n">
+        <v>0.3535533905932738</v>
+      </c>
+      <c r="B89" s="11" t="n">
+        <v>0.3535533905932738</v>
+      </c>
+      <c r="C89" s="11" t="n">
+        <v>-0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="11" t="n">
+        <v>3.061616997868384e-17</v>
+      </c>
+      <c r="B90" s="11" t="n">
+        <v>0.5000000000000001</v>
+      </c>
+      <c r="C90" s="11" t="n">
+        <v>-0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="11" t="n">
+        <v>-0.3535533905932738</v>
+      </c>
+      <c r="B91" s="11" t="n">
+        <v>0.3535533905932738</v>
+      </c>
+      <c r="C91" s="11" t="n">
+        <v>-0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="11" t="n">
+        <v>-0.5000000000000001</v>
+      </c>
+      <c r="B92" s="11" t="n">
+        <v>6.123233995736767e-17</v>
+      </c>
+      <c r="C92" s="11" t="n">
+        <v>-0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="11" t="n">
+        <v>-0.3535533905932739</v>
+      </c>
+      <c r="B93" s="11" t="n">
+        <v>-0.3535533905932738</v>
+      </c>
+      <c r="C93" s="11" t="n">
+        <v>-0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="11" t="n">
+        <v>-9.184850993605151e-17</v>
+      </c>
+      <c r="B94" s="11" t="n">
+        <v>-0.5000000000000001</v>
+      </c>
+      <c r="C94" s="11" t="n">
+        <v>-0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="11" t="n">
+        <v>0.3535533905932737</v>
+      </c>
+      <c r="B95" s="11" t="n">
+        <v>-0.3535533905932739</v>
+      </c>
+      <c r="C95" s="11" t="n">
+        <v>-0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="11" t="n">
+        <v>0.1736481776669304</v>
+      </c>
+      <c r="B96" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C96" s="11" t="n">
+        <v>-0.984807753012208</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="11" t="n">
+        <v>-0.1736481776669304</v>
+      </c>
+      <c r="B97" s="11" t="n">
+        <v>2.126576849575772e-17</v>
+      </c>
+      <c r="C97" s="11" t="n">
+        <v>-0.984807753012208</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B98" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C98" s="11" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -22383,7 +23486,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="10:14 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -22487,7 +23590,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="10:14 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -22596,7 +23699,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="1" sqref="10:14 H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -22748,7 +23851,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="10:14 C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -22900,7 +24003,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -22954,7 +24057,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -23008,7 +24111,7 @@
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>

</xml_diff>

<commit_message>
Speed ups to the code have been made by assigning sparse matrix terms individually not by slice, enumerate instead of using length and range, and importing functions rather than calling through modules. There were errors found in remove doubles and duplicate check during this speeding up and these have now been fixed.
</commit_message>
<xml_diff>
--- a/ParameterIndependent/InputSheet.xlsx
+++ b/ParameterIndependent/InputSheet.xlsx
@@ -12204,10 +12204,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -12255,7 +12255,7 @@
         </is>
       </c>
       <c r="C2" s="14" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" ht="35.4" customHeight="1" s="12">
@@ -12457,7 +12457,7 @@
       </c>
       <c r="C15" s="14" t="inlineStr">
         <is>
-          <t>MultiPerfRefNoBoxOffCentre</t>
+          <t>twoPerfRefNoBoxOffCentre</t>
         </is>
       </c>
     </row>
@@ -12610,6 +12610,23 @@
       </c>
       <c r="C25" s="14" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="26" ht="46.25" customHeight="1" s="12">
+      <c r="A26" s="13" t="inlineStr">
+        <is>
+          <t>String representation of the reflective obstacles</t>
+        </is>
+      </c>
+      <c r="B26" s="14" t="inlineStr">
+        <is>
+          <t>Obstr</t>
+        </is>
+      </c>
+      <c r="C26" s="11" t="inlineStr">
+        <is>
+          <t>Ob02Ob03</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -64444,7 +64461,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -64603,8 +64620,8 @@
   </sheetPr>
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -65056,8 +65073,8 @@
   </sheetPr>
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>

</xml_diff>

<commit_message>
update to paramter table
</commit_message>
<xml_diff>
--- a/ParameterIndependent/InputSheet.xlsx
+++ b/ParameterIndependent/InputSheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AngleSpacing" sheetId="1" state="visible" r:id="rId1"/>
@@ -522,8 +522,8 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="I7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -670,7 +670,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -936,7 +936,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -1312,7 +1312,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -1820,7 +1820,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -2460,7 +2460,7 @@
   <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -3441,7 +3441,7 @@
   <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -4543,7 +4543,7 @@
   <dimension ref="A1:C136"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -6063,7 +6063,7 @@
   <dimension ref="A1:C149"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -7726,7 +7726,7 @@
   <dimension ref="A1:C192"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -9862,7 +9862,7 @@
   <dimension ref="A1:C211"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -12206,8 +12206,8 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P7" activeCellId="0" sqref="P7"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P7" activeCellId="1" sqref="1:1 P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -12330,10 +12330,10 @@
         </is>
       </c>
       <c r="C7" s="14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" ht="28.8" customHeight="1" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="28.8" customFormat="1" customHeight="1" s="11">
       <c r="A8" s="13" t="inlineStr">
         <is>
           <t>Transmitter location</t>
@@ -12344,7 +12344,6 @@
           <t>Tx</t>
         </is>
       </c>
-      <c r="C8" s="11" t="n"/>
       <c r="D8" s="11" t="n">
         <v>0.1</v>
       </c>
@@ -12427,7 +12426,7 @@
         </is>
       </c>
       <c r="C13" s="14" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" ht="14.4" customHeight="1" s="12">
@@ -12458,7 +12457,7 @@
       </c>
       <c r="C15" s="14" t="inlineStr">
         <is>
-          <t>twoPerfRefNoBoxOffCentre</t>
+          <t>MultiPerfRefBoxOffCentre</t>
         </is>
       </c>
     </row>
@@ -12642,7 +12641,7 @@
   <dimension ref="A1:C244"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -15350,7 +15349,7 @@
   <dimension ref="A1:C282"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -18476,7 +18475,7 @@
   <dimension ref="A1:C337"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -22207,7 +22206,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -22473,7 +22472,7 @@
   <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -23575,7 +23574,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -23951,7 +23950,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -24459,7 +24458,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -25099,7 +25098,7 @@
   <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -26080,7 +26079,7 @@
   <dimension ref="A1:C300"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -29404,7 +29403,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="1" sqref="1:1 G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -29508,7 +29507,7 @@
   <dimension ref="A1:C3153"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -64212,10 +64211,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -64224,83 +64223,76 @@
     <col width="8.67" customWidth="1" style="11" min="2" max="1025"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.4" customHeight="1" s="12">
+    <row r="1" ht="13.8" customHeight="1" s="12">
+      <c r="A1" s="11" t="inlineStr">
+        <is>
+          <t>Wood Coeffs</t>
+        </is>
+      </c>
       <c r="B1" s="11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C1" s="20" t="inlineStr">
+        <is>
+          <t>3.825+0.013j</t>
+        </is>
+      </c>
+      <c r="D1" s="11" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E1" s="11" t="inlineStr">
+        <is>
+          <t>(0.8855885559191065+0.003942667577037837j)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="14.4" customHeight="1" s="12">
+      <c r="B2" s="11" t="inlineStr">
         <is>
           <t>mur</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C2" s="11" t="inlineStr">
         <is>
           <t>epsr</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D2" s="11" t="inlineStr">
         <is>
           <t>sigma</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E2" s="11" t="inlineStr">
         <is>
           <t>Znobrat</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F2" s="11" t="inlineStr">
         <is>
           <t>refindex</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="14.4" customHeight="1" s="12">
-      <c r="A2" s="11" t="inlineStr">
+    <row r="3" ht="14.4" customHeight="1" s="12">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t>OuterBoundary1</t>
         </is>
       </c>
-      <c r="B2" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="11" t="inlineStr">
+      <c r="B3" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
-        </is>
-      </c>
-      <c r="F2" s="11" t="inlineStr">
-        <is>
-          <t>0j</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="14.4" customHeight="1" s="12">
-      <c r="A3" s="11" t="inlineStr">
-        <is>
-          <t>OuterBoundary2</t>
-        </is>
-      </c>
-      <c r="B3" s="11" t="inlineStr">
-        <is>
-          <t>0j</t>
-        </is>
-      </c>
-      <c r="C3" s="20" t="inlineStr">
-        <is>
-          <t>0j</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="inlineStr">
-        <is>
-          <t>0j</t>
-        </is>
-      </c>
-      <c r="E3" s="20" t="inlineStr">
-        <is>
-          <t>0j</t>
+          <t>(0.8855885559191065+0.003942667577037837j)</t>
         </is>
       </c>
       <c r="F3" s="11" t="inlineStr">
@@ -64312,170 +64304,198 @@
     <row r="4" ht="14.4" customHeight="1" s="12">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundary3</t>
+          <t>OuterBoundary2</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(3+0j)</t>
         </is>
       </c>
       <c r="C4" s="20" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(3.825+0.013j)</t>
         </is>
       </c>
       <c r="D4" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(0.0001+0j)</t>
         </is>
       </c>
-      <c r="E4" s="11" t="inlineStr">
+      <c r="E4" s="20" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(0.8855885559191065+0.003942667577037837j)</t>
         </is>
       </c>
       <c r="F4" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(11.475000000000001+0.039j)</t>
         </is>
       </c>
     </row>
     <row r="5" ht="14.4" customHeight="1" s="12">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundary4</t>
+          <t>OuterBoundary3</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(3+0j)</t>
         </is>
       </c>
       <c r="C5" s="20" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(3.825+0.013j)</t>
         </is>
       </c>
       <c r="D5" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(0.0001+0j)</t>
         </is>
       </c>
       <c r="E5" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(0.8855885559191065+0.003942667577037837j)</t>
         </is>
       </c>
       <c r="F5" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(11.475000000000001+0.039j)</t>
         </is>
       </c>
     </row>
     <row r="6" ht="14.4" customHeight="1" s="12">
       <c r="A6" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundary5</t>
+          <t>OuterBoundary4</t>
         </is>
       </c>
       <c r="B6" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(3+0j)</t>
         </is>
       </c>
       <c r="C6" s="20" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(3.825+0.013j)</t>
         </is>
       </c>
       <c r="D6" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(0.0001+0j)</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(0.8855885559191065+0.003942667577037837j)</t>
         </is>
       </c>
       <c r="F6" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(11.475000000000001+0.039j)</t>
         </is>
       </c>
     </row>
     <row r="7" ht="14.4" customHeight="1" s="12">
       <c r="A7" s="11" t="inlineStr">
         <is>
-          <t>OuterBoundary6</t>
+          <t>OuterBoundary5</t>
         </is>
       </c>
       <c r="B7" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(3+0j)</t>
         </is>
       </c>
       <c r="C7" s="20" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(3.825+0.013j)</t>
         </is>
       </c>
       <c r="D7" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(0.0001+0j)</t>
         </is>
       </c>
-      <c r="E7" s="20" t="inlineStr">
+      <c r="E7" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(0.8855885559191065+0.003942667577037837j)</t>
         </is>
       </c>
       <c r="F7" s="11" t="inlineStr">
         <is>
-          <t>0j</t>
+          <t>(11.475000000000001+0.039j)</t>
         </is>
       </c>
     </row>
     <row r="8" ht="14.4" customHeight="1" s="12">
       <c r="A8" s="11" t="inlineStr">
         <is>
-          <t>Obstacle1</t>
+          <t>OuterBoundary6</t>
         </is>
       </c>
-      <c r="B8" s="11" t="n"/>
-      <c r="C8" s="11" t="n"/>
-      <c r="D8" s="11" t="n"/>
-      <c r="E8" s="11" t="n"/>
-      <c r="F8" s="11" t="n"/>
-    </row>
-    <row r="10" ht="13.8" customHeight="1" s="12"/>
-    <row r="11" ht="13.8" customHeight="1" s="12">
-      <c r="A11" s="11" t="inlineStr">
+      <c r="B8" s="11" t="inlineStr">
         <is>
-          <t>Wood Coeffs</t>
+          <t>(3+0j)</t>
         </is>
       </c>
-      <c r="B11" s="11" t="inlineStr">
+      <c r="C8" s="20" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>(3.825+0.013j)</t>
         </is>
       </c>
-      <c r="C11" s="20" t="inlineStr">
+      <c r="D8" s="11" t="inlineStr">
         <is>
-          <t>3.825+0.013j</t>
+          <t>(0.0001+0j)</t>
         </is>
       </c>
-      <c r="D11" s="11" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="E11" s="11" t="inlineStr">
+      <c r="E8" s="20" t="inlineStr">
         <is>
           <t>(0.8855885559191065+0.003942667577037837j)</t>
         </is>
       </c>
-    </row>
-    <row r="19" ht="13.8" customHeight="1" s="12"/>
+      <c r="F8" s="11" t="inlineStr">
+        <is>
+          <t>(11.475000000000001+0.039j)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="14.4" customHeight="1" s="12">
+      <c r="A9" s="11" t="inlineStr">
+        <is>
+          <t>Obstacle1</t>
+        </is>
+      </c>
+      <c r="B9" s="11" t="inlineStr">
+        <is>
+          <t>(3+0j)</t>
+        </is>
+      </c>
+      <c r="C9" s="11" t="inlineStr">
+        <is>
+          <t>(3.825+0.013j)</t>
+        </is>
+      </c>
+      <c r="D9" s="11" t="inlineStr">
+        <is>
+          <t>(0.0001+0j)</t>
+        </is>
+      </c>
+      <c r="E9" s="11" t="inlineStr">
+        <is>
+          <t>(0.8855885559191065+0.003942667577037837j)</t>
+        </is>
+      </c>
+      <c r="F9" s="11" t="inlineStr">
+        <is>
+          <t>(11.475000000000001+0.039j)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="13.8" customHeight="1" s="12"/>
+    <row r="12" ht="13.8" customHeight="1" s="12"/>
+    <row r="20" ht="13.8" customHeight="1" s="12"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -64492,7 +64512,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="1" sqref="1:1 K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -64652,7 +64672,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="1:1 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -64997,7 +65017,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -65051,7 +65071,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
@@ -65105,7 +65125,7 @@
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+      <selection pane="topLeft" activeCell="D45" activeCellId="1" sqref="1:1 D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>

</xml_diff>